<commit_message>
Se agregaron las variables por defecto, estas se colocan directamente en el excel
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -3651,184 +3651,817 @@
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="37">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>nayibis</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>none</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>morelo</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>marimon</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>cc</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">14/01/1971 </t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>40925684</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">14/01/1971 +</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ama de casa</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nivel 1</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">comfaguajira pgp oncologia subsidiado </t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ninguno de los anteriores </t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">no definido </t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">riohacha </t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3226754735 </t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ama de casa+</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nivel 1+</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comfaguajira pgp oncologia subsidiado +</t>
+        </is>
+      </c>
+      <c r="L4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ninguno de los anteriores +</t>
+        </is>
+      </c>
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no definido+</t>
+        </is>
+      </c>
+      <c r="N4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">riohacha +</t>
+        </is>
+      </c>
+      <c r="O4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3226754735 +</t>
+        </is>
+      </c>
+      <c r="P4" s="0" t="inlineStr">
         <is>
           <t>na</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" s="0" t="inlineStr">
         <is>
           <t>c509</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="S4" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="AD4" t="inlineStr">
+      <c r="T4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="U4" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="V4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Y4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Z4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="AD4" s="0" t="inlineStr">
         <is>
           <t>19/04/2021</t>
         </is>
       </c>
-      <c r="EJ4" t="inlineStr">
+      <c r="AE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AF4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AN4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EK4" t="inlineStr">
+      <c r="AO4" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AP4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AR4" s="0" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AS4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AV4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AW4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AX4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AY4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AZ4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BA4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BB4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CB4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CW4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CX4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CY4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DA4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DB4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DJ4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DP4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DS4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DV4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DW4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DY4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EA4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EB4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ED4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EE4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EH4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EJ4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EL4" t="inlineStr">
+      <c r="EK4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EL4" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EM4" t="inlineStr">
+      <c r="EM4" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EN4" t="inlineStr">
+      <c r="EN4" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EO4" t="inlineStr">
+      <c r="EO4" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EP4" t="inlineStr">
+      <c r="EP4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EQ4" t="inlineStr">
+      <c r="EQ4" s="0" t="inlineStr">
         <is>
           <t>23/03/2021</t>
         </is>
       </c>
-      <c r="ER4" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="ES4" t="inlineStr">
+      <c r="ER4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES4" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="ET4" t="inlineStr">
+      <c r="ET4" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="EU4" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EV4" t="inlineStr">
+      <c r="EU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EW4" t="inlineStr">
+      <c r="EW4" s="0" t="inlineStr">
         <is>
           <t>25/01/2021</t>
         </is>
       </c>
-      <c r="EX4" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EY4" t="inlineStr">
+      <c r="EX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EY4" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EZ4" t="inlineStr">
-        <is>
-          <t>98</t>
+      <c r="EZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FA4" s="0" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="FB4" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="FC4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FD4" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FE4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FF4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FG4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FJ4" s="0" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego la funcionalidad de poder leer varios historiales clinicos y poderlos consignar en el excel
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -729,7 +729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:FJ4"/>
+  <dimension ref="A1:FJ6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="EV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="EY8" activeCellId="0" sqref="EY8"/>
@@ -3653,813 +3653,2443 @@
     <row r="4" ht="13.8" customHeight="1" s="37">
       <c r="A4" s="0" t="inlineStr">
         <is>
+          <t>yoraima</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>aracelly</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>mejia</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>uriana</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>cc</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>1192943668</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">19/09/1985 +</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">otras ocupaciones elementales+</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nivel 1+</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comfaguajira pgp oncologia subsidiado +</t>
+        </is>
+      </c>
+      <c r="L4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ninguno de los anteriores +</t>
+        </is>
+      </c>
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no definido+</t>
+        </is>
+      </c>
+      <c r="N4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">riohacha +</t>
+        </is>
+      </c>
+      <c r="O4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3234440935 +</t>
+        </is>
+      </c>
+      <c r="P4" s="0" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="Q4" s="0" t="inlineStr">
+        <is>
+          <t>c910</t>
+        </is>
+      </c>
+      <c r="R4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="S4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="T4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="U4" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="V4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Y4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Z4" s="0" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="AD4" s="0" t="inlineStr">
+        <is>
+          <t>30/04/2021</t>
+        </is>
+      </c>
+      <c r="AE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AF4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AN4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO4" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AP4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AR4" s="0" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AS4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AV4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AW4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AX4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AY4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AZ4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BA4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BB4" s="0" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CB4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CW4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CX4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CY4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DA4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DB4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DD4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DE4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DJ4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DK4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DL4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DM4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DN4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DO4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DP4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DQ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DR4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DS4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DT4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DV4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DW4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DY4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EA4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EB4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EC4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ED4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EE4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EF4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EG4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EH4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EJ4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EK4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EL4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EM4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EN4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EO4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EP4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EQ4" s="0" t="inlineStr">
+        <is>
+          <t>15/04/2021</t>
+        </is>
+      </c>
+      <c r="ER4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="ET4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">y hora de </t>
+        </is>
+      </c>
+      <c r="EU4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EW4" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve">y hora de </t>
+        </is>
+      </c>
+      <c r="EX4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EY4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EZ4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FA4" s="0" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="FB4" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="FC4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FD4" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FE4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FF4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FG4" s="0" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FH4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FI4" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FJ4" s="0" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
           <t>nayibis</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>none</t>
         </is>
       </c>
-      <c r="C4" s="0" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>morelo</t>
         </is>
       </c>
-      <c r="D4" s="0" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>marimon</t>
         </is>
       </c>
-      <c r="E4" s="0" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>cc</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>40925684</t>
         </is>
       </c>
-      <c r="G4" s="0" t="inlineStr">
+      <c r="G5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">14/01/1971  </t>
         </is>
       </c>
-      <c r="H4" s="0" t="inlineStr">
+      <c r="H5" s="0" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="I4" s="0" t="inlineStr">
+      <c r="I5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">ama de casa </t>
         </is>
       </c>
-      <c r="J4" s="0" t="inlineStr">
+      <c r="J5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">nivel 1 </t>
         </is>
       </c>
-      <c r="K4" s="0" t="inlineStr">
+      <c r="K5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">comfaguajira pgp oncologia subsidiado  </t>
         </is>
       </c>
-      <c r="L4" s="0" t="inlineStr">
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">ninguno de los anteriores  </t>
         </is>
       </c>
-      <c r="M4" s="0" t="inlineStr">
+      <c r="M5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">no definido </t>
         </is>
       </c>
-      <c r="N4" s="0" t="inlineStr">
+      <c r="N5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">riohacha  </t>
         </is>
       </c>
-      <c r="O4" s="0" t="inlineStr">
+      <c r="O5" s="0" t="inlineStr">
         <is>
           <t xml:space="preserve">3226754735  </t>
         </is>
       </c>
-      <c r="P4" s="0" t="inlineStr">
+      <c r="P5" s="0" t="inlineStr">
         <is>
           <t>na</t>
         </is>
       </c>
-      <c r="Q4" s="0" t="inlineStr">
+      <c r="Q5" s="0" t="inlineStr">
         <is>
           <t>c509</t>
         </is>
       </c>
-      <c r="R4" s="0" t="inlineStr">
+      <c r="R5" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="S4" s="0" t="inlineStr">
+      <c r="S5" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="T4" s="0" t="inlineStr">
+      <c r="T5" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="U4" s="0" t="inlineStr">
+      <c r="U5" s="0" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="V4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="Y4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="Z4" s="0" t="inlineStr">
+      <c r="V5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Y5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Z5" s="0" t="inlineStr">
         <is>
           <t>1800-01-01</t>
         </is>
       </c>
-      <c r="AD4" s="0" t="inlineStr">
+      <c r="AD5" s="0" t="inlineStr">
         <is>
           <t>19/04/2021</t>
         </is>
       </c>
-      <c r="AE4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AF4" s="0" t="inlineStr">
+      <c r="AE5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AF5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="AG4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AH4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AI4" s="0" t="inlineStr">
+      <c r="AG5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AH5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="AJ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AK4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AL4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AM4" s="0" t="inlineStr">
+      <c r="AJ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="AN4" s="0" t="inlineStr">
+      <c r="AN5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AO4" s="0" t="inlineStr">
+      <c r="AO5" s="0" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="AP4" s="0" t="inlineStr">
+      <c r="AP5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AQ4" s="0" t="inlineStr">
+      <c r="AQ5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="AR4" s="0" t="inlineStr">
+      <c r="AR5" s="0" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="AS4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AT4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AU4" s="0" t="inlineStr">
+      <c r="AS5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="AV4" s="0" t="inlineStr">
+      <c r="AV5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="AW4" s="0" t="inlineStr">
+      <c r="AW5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="AX4" s="0" t="inlineStr">
+      <c r="AX5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="AY4" s="0" t="inlineStr">
+      <c r="AY5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="AZ4" s="0" t="inlineStr">
+      <c r="AZ5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="BA4" s="0" t="inlineStr">
+      <c r="BA5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="BB4" s="0" t="inlineStr">
+      <c r="BB5" s="0" t="inlineStr">
         <is>
           <t>97</t>
         </is>
       </c>
-      <c r="BC4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BD4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BE4" s="0" t="inlineStr">
+      <c r="BC5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="BF4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BG4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BH4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BI4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BJ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BK4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BL4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BM4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BN4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BO4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BP4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BQ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BR4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BS4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BT4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BU4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BV4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BW4" s="0" t="inlineStr">
+      <c r="BF5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="BX4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BY4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BZ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CA4" s="0" t="inlineStr">
+      <c r="BX5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="CB4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CC4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CD4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CE4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CF4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CG4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CH4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CI4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CJ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CK4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CL4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CM4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CN4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CO4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CP4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CQ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CR4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CS4" s="0" t="inlineStr">
+      <c r="CB5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="CT4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CU4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CV4" s="0" t="inlineStr">
+      <c r="CT5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="CW4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CX4" s="0" t="inlineStr">
+      <c r="CW5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CX5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="CY4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CZ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DA4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DB4" s="0" t="inlineStr">
+      <c r="CY5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CZ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DA5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DB5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="DC4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DD4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DE4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DF4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DG4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DH4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DI4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DJ4" s="0" t="inlineStr">
+      <c r="DC5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DD5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DE5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DF5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DG5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DH5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DI5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DJ5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="DK4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DL4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DM4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DN4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DO4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DP4" s="0" t="inlineStr">
+      <c r="DK5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DL5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DM5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DN5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DO5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DP5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="DQ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DR4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DS4" s="0" t="inlineStr">
+      <c r="DQ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DR5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DS5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="DT4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DU4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DV4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DW4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DX4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="DY4" s="0" t="inlineStr">
+      <c r="DT5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DU5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DV5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DW5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DX5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DY5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="DZ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EA4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EB4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EC4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="ED4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EE4" s="0" t="inlineStr">
+      <c r="DZ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EA5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EB5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EC5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ED5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EE5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="EF4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EG4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EH4" s="0" t="inlineStr">
+      <c r="EF5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EG5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EH5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="EI4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EJ4" s="0" t="inlineStr">
+      <c r="EI5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EJ5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EK4" s="0" t="inlineStr">
+      <c r="EK5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EL4" s="0" t="inlineStr">
+      <c r="EL5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EM4" s="0" t="inlineStr">
+      <c r="EM5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EN4" s="0" t="inlineStr">
+      <c r="EN5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EO4" s="0" t="inlineStr">
+      <c r="EO5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="EP4" s="0" t="inlineStr">
+      <c r="EP5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EQ4" s="0" t="inlineStr">
+      <c r="EQ5" s="0" t="inlineStr">
         <is>
           <t>23/03/2021</t>
         </is>
       </c>
-      <c r="ER4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="ES4" s="0" t="inlineStr">
+      <c r="ER5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES5" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="ET4" s="0" t="inlineStr">
+      <c r="ET5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="EU4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EV4" s="0" t="inlineStr">
+      <c r="EU5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EW4" s="0" t="inlineStr">
+      <c r="EW5" s="0" t="inlineStr">
         <is>
           <t>25/01/2021</t>
         </is>
       </c>
-      <c r="EX4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EY4" s="0" t="inlineStr">
+      <c r="EX5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EY5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EZ4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="FA4" s="0" t="inlineStr">
+      <c r="EZ5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FA5" s="0" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="FB4" s="0" t="inlineStr">
+      <c r="FB5" s="0" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="FC4" s="0" t="inlineStr">
+      <c r="FC5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="FD4" s="0" t="inlineStr">
+      <c r="FD5" s="0" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="FE4" s="0" t="inlineStr">
+      <c r="FE5" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="FF4" s="0" t="inlineStr">
+      <c r="FF5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="FG4" s="0" t="inlineStr">
+      <c r="FG5" s="0" t="inlineStr">
         <is>
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="FH4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="FI4" s="0" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="FJ4" s="0" t="inlineStr">
+      <c r="FH5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FI5" s="0" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FJ5" s="0" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>warner</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>chistian</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>montenegro</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>barros</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>cc</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>84046881</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10/02/1989 +</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">otras ocupaciones elementales+</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cotizante nivel 1+</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">comfaguajira pgp oncologia subsidiado +</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ninguno de los anteriores +</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no definido+</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">maicao +</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3185218372 +</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>na</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>c859</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>30/04/2021</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BX6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CB6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CT6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CW6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CX6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CY6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CZ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DA6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DB6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DC6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DD6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DE6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DF6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DG6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DH6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DI6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DJ6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DK6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DL6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DM6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DN6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DO6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DP6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DQ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DR6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DS6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DT6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DU6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DV6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DW6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DX6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DY6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DZ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EA6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EB6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EC6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ED6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EE6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EF6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EG6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EH6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EI6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EJ6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EK6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EL6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EM6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EN6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EO6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EP6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EQ6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="ER6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="ET6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EU6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EW6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EX6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EY6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EZ6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FA6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="FB6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="FC6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FD6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FE6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FF6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FG6" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FH6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FI6" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FJ6" t="inlineStr">
         <is>
           <t>2021-01-01</t>
         </is>

</xml_diff>

<commit_message>
arreglo de formato de las fechas que se tienen hasta el momento, creacion de csv de las eps, en espera para confirmar codigo de las eps repetidas
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -166,6 +166,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -279,9 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
@@ -770,13 +770,15 @@
   </sheetPr>
   <dimension ref="A1:FX24"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="FD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:FJ6"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="FJ4" activeCellId="0" sqref="A4:FJ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="18.47" customWidth="1" style="41" min="7" max="7"/>
+    <col width="12.96" customWidth="1" style="41" min="1" max="6"/>
+    <col width="12.96" customWidth="1" style="41" min="7" max="7"/>
+    <col width="12.96" customWidth="1" style="41" min="8" max="166"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1" s="42">
@@ -3827,7 +3829,7 @@
       </c>
       <c r="AD4" s="80" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>2021-04-30</t>
         </is>
       </c>
       <c r="AE4" s="80" t="inlineStr">
@@ -4660,7 +4662,7 @@
       </c>
       <c r="AD5" s="80" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>2021-04-30</t>
         </is>
       </c>
       <c r="AE5" s="80" t="inlineStr">
@@ -5245,7 +5247,7 @@
       </c>
       <c r="EQ5" s="80" t="inlineStr">
         <is>
-          <t>15/04/2021</t>
+          <t>2021-04-15</t>
         </is>
       </c>
       <c r="ER5" s="80" t="inlineStr">
@@ -5493,7 +5495,7 @@
       </c>
       <c r="AD6" s="80" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>2021-04-19</t>
         </is>
       </c>
       <c r="AE6" s="80" t="inlineStr">
@@ -6078,7 +6080,7 @@
       </c>
       <c r="EQ6" s="80" t="inlineStr">
         <is>
-          <t>23/03/2021</t>
+          <t>2021-03-23</t>
         </is>
       </c>
       <c r="ER6" s="80" t="inlineStr">
@@ -6108,7 +6110,7 @@
       </c>
       <c r="EW6" s="80" t="inlineStr">
         <is>
-          <t>25/01/2021</t>
+          <t>2021-01-25</t>
         </is>
       </c>
       <c r="EX6" s="80" t="inlineStr">
@@ -6366,7 +6368,6 @@
       <c r="D8" s="41" t="n"/>
       <c r="E8" s="41" t="n"/>
       <c r="F8" s="41" t="n"/>
-      <c r="G8" s="41" t="n"/>
       <c r="H8" s="41" t="n"/>
       <c r="I8" s="41" t="n"/>
       <c r="J8" s="41" t="n"/>
@@ -6534,7 +6535,6 @@
       <c r="D9" s="41" t="n"/>
       <c r="E9" s="41" t="n"/>
       <c r="F9" s="41" t="n"/>
-      <c r="G9" s="41" t="n"/>
       <c r="H9" s="41" t="n"/>
       <c r="I9" s="41" t="n"/>
       <c r="J9" s="41" t="n"/>
@@ -6702,7 +6702,6 @@
       <c r="D10" s="41" t="n"/>
       <c r="E10" s="41" t="n"/>
       <c r="F10" s="41" t="n"/>
-      <c r="G10" s="41" t="n"/>
       <c r="H10" s="41" t="n"/>
       <c r="I10" s="41" t="n"/>
       <c r="J10" s="41" t="n"/>
@@ -6870,7 +6869,6 @@
       <c r="D11" s="41" t="n"/>
       <c r="E11" s="41" t="n"/>
       <c r="F11" s="41" t="n"/>
-      <c r="G11" s="41" t="n"/>
       <c r="H11" s="41" t="n"/>
       <c r="I11" s="41" t="n"/>
       <c r="J11" s="41" t="n"/>
@@ -7038,7 +7036,6 @@
       <c r="D12" s="41" t="n"/>
       <c r="E12" s="41" t="n"/>
       <c r="F12" s="41" t="n"/>
-      <c r="G12" s="41" t="n"/>
       <c r="H12" s="41" t="n"/>
       <c r="I12" s="41" t="n"/>
       <c r="J12" s="41" t="n"/>
@@ -7206,7 +7203,6 @@
       <c r="D13" s="41" t="n"/>
       <c r="E13" s="41" t="n"/>
       <c r="F13" s="41" t="n"/>
-      <c r="G13" s="41" t="n"/>
       <c r="H13" s="41" t="n"/>
       <c r="I13" s="41" t="n"/>
       <c r="J13" s="41" t="n"/>
@@ -7374,7 +7370,6 @@
       <c r="D14" s="41" t="n"/>
       <c r="E14" s="41" t="n"/>
       <c r="F14" s="41" t="n"/>
-      <c r="G14" s="41" t="n"/>
       <c r="H14" s="41" t="n"/>
       <c r="I14" s="41" t="n"/>
       <c r="J14" s="41" t="n"/>
@@ -7542,7 +7537,6 @@
       <c r="D15" s="41" t="n"/>
       <c r="E15" s="41" t="n"/>
       <c r="F15" s="41" t="n"/>
-      <c r="G15" s="41" t="n"/>
       <c r="H15" s="41" t="n"/>
       <c r="I15" s="41" t="n"/>
       <c r="J15" s="41" t="n"/>
@@ -7710,7 +7704,6 @@
       <c r="D16" s="41" t="n"/>
       <c r="E16" s="41" t="n"/>
       <c r="F16" s="41" t="n"/>
-      <c r="G16" s="41" t="n"/>
       <c r="H16" s="41" t="n"/>
       <c r="I16" s="41" t="n"/>
       <c r="J16" s="41" t="n"/>
@@ -7878,7 +7871,6 @@
       <c r="D17" s="41" t="n"/>
       <c r="E17" s="41" t="n"/>
       <c r="F17" s="41" t="n"/>
-      <c r="G17" s="41" t="n"/>
       <c r="H17" s="41" t="n"/>
       <c r="I17" s="41" t="n"/>
       <c r="J17" s="41" t="n"/>
@@ -8046,7 +8038,6 @@
       <c r="D18" s="41" t="n"/>
       <c r="E18" s="41" t="n"/>
       <c r="F18" s="41" t="n"/>
-      <c r="G18" s="41" t="n"/>
       <c r="H18" s="41" t="n"/>
       <c r="I18" s="41" t="n"/>
       <c r="J18" s="41" t="n"/>
@@ -8214,7 +8205,6 @@
       <c r="D19" s="41" t="n"/>
       <c r="E19" s="41" t="n"/>
       <c r="F19" s="41" t="n"/>
-      <c r="G19" s="41" t="n"/>
       <c r="H19" s="41" t="n"/>
       <c r="I19" s="41" t="n"/>
       <c r="J19" s="41" t="n"/>
@@ -8382,7 +8372,6 @@
       <c r="D20" s="41" t="n"/>
       <c r="E20" s="41" t="n"/>
       <c r="F20" s="41" t="n"/>
-      <c r="G20" s="41" t="n"/>
       <c r="H20" s="41" t="n"/>
       <c r="I20" s="41" t="n"/>
       <c r="J20" s="41" t="n"/>
@@ -8550,7 +8539,6 @@
       <c r="D21" s="41" t="n"/>
       <c r="E21" s="41" t="n"/>
       <c r="F21" s="41" t="n"/>
-      <c r="G21" s="41" t="n"/>
       <c r="H21" s="41" t="n"/>
       <c r="I21" s="41" t="n"/>
       <c r="J21" s="41" t="n"/>
@@ -8718,7 +8706,6 @@
       <c r="D22" s="41" t="n"/>
       <c r="E22" s="41" t="n"/>
       <c r="F22" s="41" t="n"/>
-      <c r="G22" s="41" t="n"/>
       <c r="H22" s="41" t="n"/>
       <c r="I22" s="41" t="n"/>
       <c r="J22" s="41" t="n"/>
@@ -8886,7 +8873,6 @@
       <c r="D23" s="41" t="n"/>
       <c r="E23" s="41" t="n"/>
       <c r="F23" s="41" t="n"/>
-      <c r="G23" s="41" t="n"/>
       <c r="H23" s="41" t="n"/>
       <c r="I23" s="41" t="n"/>
       <c r="J23" s="41" t="n"/>
@@ -9054,7 +9040,6 @@
       <c r="D24" s="41" t="n"/>
       <c r="E24" s="41" t="n"/>
       <c r="F24" s="41" t="n"/>
-      <c r="G24" s="41" t="n"/>
       <c r="H24" s="41" t="n"/>
       <c r="I24" s="41" t="n"/>
       <c r="J24" s="41" t="n"/>
@@ -9234,7 +9219,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:FJ6 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Se agrego la seccion del resultado final
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -768,17 +768,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:FX24"/>
+  <dimension ref="A1:FX7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="FJ4" activeCellId="0" sqref="A4:FJ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="12.96" customWidth="1" style="41" min="1" max="6"/>
-    <col width="12.96" customWidth="1" style="41" min="7" max="7"/>
-    <col width="12.96" customWidth="1" style="41" min="8" max="166"/>
+    <col width="12.96" customWidth="1" style="41" min="1" max="166"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1" s="42">
@@ -4464,27 +4462,27 @@
       </c>
       <c r="FA4" s="80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>98</t>
         </is>
       </c>
       <c r="FB4" s="80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>99</t>
         </is>
       </c>
       <c r="FC4" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="FD4" s="80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="FE4" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="FF4" s="80" t="inlineStr">
@@ -4492,16 +4490,8 @@
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="FG4" s="80" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="FH4" s="80" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
+      <c r="FG4" s="80" t="inlineStr"/>
+      <c r="FH4" s="80" t="inlineStr"/>
       <c r="FI4" s="80" t="inlineStr">
         <is>
           <t>98</t>
@@ -5297,27 +5287,27 @@
       </c>
       <c r="FA5" s="80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>98</t>
         </is>
       </c>
       <c r="FB5" s="80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>99</t>
         </is>
       </c>
       <c r="FC5" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="FD5" s="80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="FE5" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="FF5" s="80" t="inlineStr">
@@ -5325,16 +5315,8 @@
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="FG5" s="80" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="FH5" s="80" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
+      <c r="FG5" s="80" t="inlineStr"/>
+      <c r="FH5" s="80" t="inlineStr"/>
       <c r="FI5" s="80" t="inlineStr">
         <is>
           <t>98</t>
@@ -6130,27 +6112,27 @@
       </c>
       <c r="FA6" s="80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>98</t>
         </is>
       </c>
       <c r="FB6" s="80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>99</t>
         </is>
       </c>
       <c r="FC6" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="FD6" s="80" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="FE6" s="80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="FF6" s="80" t="inlineStr">
@@ -6158,16 +6140,8 @@
           <t>1845-01-01</t>
         </is>
       </c>
-      <c r="FG6" s="80" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="FH6" s="80" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
+      <c r="FG6" s="80" t="inlineStr"/>
+      <c r="FH6" s="80" t="inlineStr"/>
       <c r="FI6" s="80" t="inlineStr">
         <is>
           <t>98</t>
@@ -6194,3012 +6168,26 @@
       <c r="FX6" s="79" t="n"/>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="42">
-      <c r="A7" s="41" t="n"/>
-      <c r="B7" s="41" t="n"/>
-      <c r="C7" s="41" t="n"/>
-      <c r="D7" s="41" t="n"/>
-      <c r="E7" s="41" t="n"/>
-      <c r="F7" s="41" t="n"/>
       <c r="G7" s="81" t="n"/>
-      <c r="H7" s="41" t="n"/>
-      <c r="I7" s="41" t="n"/>
-      <c r="J7" s="41" t="n"/>
       <c r="K7" s="81" t="n"/>
-      <c r="L7" s="41" t="n"/>
-      <c r="M7" s="41" t="n"/>
-      <c r="N7" s="41" t="n"/>
-      <c r="O7" s="41" t="n"/>
-      <c r="P7" s="41" t="n"/>
-      <c r="Q7" s="41" t="n"/>
-      <c r="R7" s="41" t="n"/>
-      <c r="S7" s="41" t="n"/>
-      <c r="T7" s="41" t="n"/>
-      <c r="U7" s="41" t="n"/>
-      <c r="V7" s="41" t="n"/>
-      <c r="W7" s="41" t="n"/>
-      <c r="X7" s="41" t="n"/>
-      <c r="Y7" s="41" t="n"/>
-      <c r="Z7" s="41" t="n"/>
-      <c r="AA7" s="41" t="n"/>
-      <c r="AB7" s="41" t="n"/>
-      <c r="AC7" s="41" t="n"/>
-      <c r="AD7" s="41" t="n"/>
-      <c r="AE7" s="41" t="n"/>
-      <c r="AF7" s="41" t="n"/>
-      <c r="AG7" s="41" t="n"/>
-      <c r="AH7" s="41" t="n"/>
-      <c r="AI7" s="41" t="n"/>
-      <c r="AJ7" s="41" t="n"/>
-      <c r="AK7" s="41" t="n"/>
-      <c r="AL7" s="41" t="n"/>
-      <c r="AM7" s="41" t="n"/>
-      <c r="AN7" s="41" t="n"/>
-      <c r="AO7" s="41" t="n"/>
-      <c r="AP7" s="41" t="n"/>
-      <c r="AQ7" s="41" t="n"/>
-      <c r="AR7" s="41" t="n"/>
-      <c r="AS7" s="41" t="n"/>
-      <c r="AT7" s="41" t="n"/>
-      <c r="AU7" s="41" t="n"/>
-      <c r="AV7" s="41" t="n"/>
-      <c r="AW7" s="41" t="n"/>
-      <c r="AX7" s="41" t="n"/>
-      <c r="AY7" s="41" t="n"/>
-      <c r="AZ7" s="41" t="n"/>
-      <c r="BA7" s="41" t="n"/>
-      <c r="BB7" s="41" t="n"/>
-      <c r="BC7" s="41" t="n"/>
-      <c r="BD7" s="41" t="n"/>
-      <c r="BE7" s="41" t="n"/>
-      <c r="BF7" s="41" t="n"/>
-      <c r="BG7" s="41" t="n"/>
-      <c r="BH7" s="41" t="n"/>
-      <c r="BI7" s="41" t="n"/>
-      <c r="BJ7" s="41" t="n"/>
-      <c r="BK7" s="41" t="n"/>
-      <c r="BL7" s="41" t="n"/>
-      <c r="BM7" s="41" t="n"/>
-      <c r="BN7" s="41" t="n"/>
-      <c r="BO7" s="41" t="n"/>
-      <c r="BP7" s="41" t="n"/>
-      <c r="BQ7" s="41" t="n"/>
-      <c r="BR7" s="41" t="n"/>
-      <c r="BS7" s="41" t="n"/>
-      <c r="BT7" s="41" t="n"/>
-      <c r="BU7" s="41" t="n"/>
-      <c r="BV7" s="41" t="n"/>
-      <c r="BW7" s="41" t="n"/>
-      <c r="BX7" s="41" t="n"/>
-      <c r="BY7" s="41" t="n"/>
-      <c r="BZ7" s="41" t="n"/>
-      <c r="CA7" s="41" t="n"/>
-      <c r="CB7" s="41" t="n"/>
-      <c r="CC7" s="41" t="n"/>
-      <c r="CD7" s="41" t="n"/>
-      <c r="CE7" s="41" t="n"/>
-      <c r="CF7" s="41" t="n"/>
-      <c r="CG7" s="41" t="n"/>
-      <c r="CH7" s="41" t="n"/>
-      <c r="CI7" s="41" t="n"/>
-      <c r="CJ7" s="41" t="n"/>
-      <c r="CK7" s="41" t="n"/>
-      <c r="CL7" s="41" t="n"/>
-      <c r="CM7" s="41" t="n"/>
-      <c r="CN7" s="41" t="n"/>
-      <c r="CO7" s="41" t="n"/>
-      <c r="CP7" s="41" t="n"/>
-      <c r="CQ7" s="41" t="n"/>
-      <c r="CR7" s="41" t="n"/>
-      <c r="CS7" s="41" t="n"/>
-      <c r="CT7" s="41" t="n"/>
-      <c r="CU7" s="41" t="n"/>
-      <c r="CV7" s="41" t="n"/>
-      <c r="CW7" s="41" t="n"/>
-      <c r="CX7" s="41" t="n"/>
-      <c r="CY7" s="41" t="n"/>
-      <c r="CZ7" s="41" t="n"/>
-      <c r="DA7" s="41" t="n"/>
-      <c r="DB7" s="41" t="n"/>
-      <c r="DC7" s="41" t="n"/>
-      <c r="DD7" s="41" t="n"/>
-      <c r="DE7" s="41" t="n"/>
-      <c r="DF7" s="41" t="n"/>
-      <c r="DG7" s="41" t="n"/>
-      <c r="DH7" s="41" t="n"/>
-      <c r="DI7" s="41" t="n"/>
-      <c r="DJ7" s="41" t="n"/>
-      <c r="DK7" s="41" t="n"/>
-      <c r="DL7" s="41" t="n"/>
-      <c r="DM7" s="41" t="n"/>
-      <c r="DN7" s="41" t="n"/>
-      <c r="DO7" s="41" t="n"/>
-      <c r="DP7" s="41" t="n"/>
-      <c r="DQ7" s="41" t="n"/>
-      <c r="DR7" s="41" t="n"/>
-      <c r="DS7" s="41" t="n"/>
-      <c r="DT7" s="41" t="n"/>
-      <c r="DU7" s="41" t="n"/>
-      <c r="DV7" s="41" t="n"/>
-      <c r="DW7" s="41" t="n"/>
-      <c r="DX7" s="41" t="n"/>
-      <c r="DY7" s="41" t="n"/>
-      <c r="DZ7" s="41" t="n"/>
-      <c r="EA7" s="41" t="n"/>
-      <c r="EB7" s="41" t="n"/>
-      <c r="EC7" s="41" t="n"/>
-      <c r="ED7" s="41" t="n"/>
-      <c r="EE7" s="41" t="n"/>
-      <c r="EF7" s="41" t="n"/>
-      <c r="EG7" s="41" t="n"/>
-      <c r="EH7" s="41" t="n"/>
-      <c r="EI7" s="41" t="n"/>
-      <c r="EJ7" s="41" t="n"/>
-      <c r="EK7" s="41" t="n"/>
-      <c r="EL7" s="41" t="n"/>
-      <c r="EM7" s="41" t="n"/>
-      <c r="EN7" s="41" t="n"/>
-      <c r="EO7" s="41" t="n"/>
-      <c r="EP7" s="41" t="n"/>
-      <c r="EQ7" s="41" t="n"/>
-      <c r="ER7" s="41" t="n"/>
-      <c r="ES7" s="41" t="n"/>
-      <c r="ET7" s="41" t="n"/>
-      <c r="EU7" s="41" t="n"/>
-      <c r="EV7" s="41" t="n"/>
-      <c r="EW7" s="41" t="n"/>
-      <c r="EX7" s="41" t="n"/>
-      <c r="EY7" s="41" t="n"/>
-      <c r="EZ7" s="41" t="n"/>
-      <c r="FA7" s="41" t="n"/>
-      <c r="FB7" s="41" t="n"/>
-      <c r="FC7" s="41" t="n"/>
-      <c r="FD7" s="41" t="n"/>
-      <c r="FE7" s="41" t="n"/>
-      <c r="FF7" s="41" t="n"/>
-      <c r="FG7" s="41" t="n"/>
-      <c r="FH7" s="41" t="n"/>
-      <c r="FI7" s="41" t="n"/>
-      <c r="FJ7" s="41" t="n"/>
     </row>
-    <row r="8" ht="13.8" customHeight="1" s="42">
-      <c r="A8" s="41" t="n"/>
-      <c r="B8" s="41" t="n"/>
-      <c r="C8" s="41" t="n"/>
-      <c r="D8" s="41" t="n"/>
-      <c r="E8" s="41" t="n"/>
-      <c r="F8" s="41" t="n"/>
-      <c r="H8" s="41" t="n"/>
-      <c r="I8" s="41" t="n"/>
-      <c r="J8" s="41" t="n"/>
-      <c r="K8" s="41" t="n"/>
-      <c r="L8" s="41" t="n"/>
-      <c r="M8" s="41" t="n"/>
-      <c r="N8" s="41" t="n"/>
-      <c r="O8" s="41" t="n"/>
-      <c r="P8" s="41" t="n"/>
-      <c r="Q8" s="41" t="n"/>
-      <c r="R8" s="41" t="n"/>
-      <c r="S8" s="41" t="n"/>
-      <c r="T8" s="41" t="n"/>
-      <c r="U8" s="41" t="n"/>
-      <c r="V8" s="41" t="n"/>
-      <c r="W8" s="41" t="n"/>
-      <c r="X8" s="41" t="n"/>
-      <c r="Y8" s="41" t="n"/>
-      <c r="Z8" s="41" t="n"/>
-      <c r="AA8" s="41" t="n"/>
-      <c r="AB8" s="41" t="n"/>
-      <c r="AC8" s="41" t="n"/>
-      <c r="AD8" s="41" t="n"/>
-      <c r="AE8" s="41" t="n"/>
-      <c r="AF8" s="41" t="n"/>
-      <c r="AG8" s="41" t="n"/>
-      <c r="AH8" s="41" t="n"/>
-      <c r="AI8" s="41" t="n"/>
-      <c r="AJ8" s="41" t="n"/>
-      <c r="AK8" s="41" t="n"/>
-      <c r="AL8" s="41" t="n"/>
-      <c r="AM8" s="41" t="n"/>
-      <c r="AN8" s="41" t="n"/>
-      <c r="AO8" s="41" t="n"/>
-      <c r="AP8" s="41" t="n"/>
-      <c r="AQ8" s="41" t="n"/>
-      <c r="AR8" s="41" t="n"/>
-      <c r="AS8" s="41" t="n"/>
-      <c r="AT8" s="41" t="n"/>
-      <c r="AU8" s="41" t="n"/>
-      <c r="AV8" s="41" t="n"/>
-      <c r="AW8" s="41" t="n"/>
-      <c r="AX8" s="41" t="n"/>
-      <c r="AY8" s="41" t="n"/>
-      <c r="AZ8" s="41" t="n"/>
-      <c r="BA8" s="41" t="n"/>
-      <c r="BB8" s="41" t="n"/>
-      <c r="BC8" s="41" t="n"/>
-      <c r="BD8" s="41" t="n"/>
-      <c r="BE8" s="41" t="n"/>
-      <c r="BF8" s="41" t="n"/>
-      <c r="BG8" s="41" t="n"/>
-      <c r="BH8" s="41" t="n"/>
-      <c r="BI8" s="41" t="n"/>
-      <c r="BJ8" s="41" t="n"/>
-      <c r="BK8" s="41" t="n"/>
-      <c r="BL8" s="41" t="n"/>
-      <c r="BM8" s="41" t="n"/>
-      <c r="BN8" s="41" t="n"/>
-      <c r="BO8" s="41" t="n"/>
-      <c r="BP8" s="41" t="n"/>
-      <c r="BQ8" s="41" t="n"/>
-      <c r="BR8" s="41" t="n"/>
-      <c r="BS8" s="41" t="n"/>
-      <c r="BT8" s="41" t="n"/>
-      <c r="BU8" s="41" t="n"/>
-      <c r="BV8" s="41" t="n"/>
-      <c r="BW8" s="41" t="n"/>
-      <c r="BX8" s="41" t="n"/>
-      <c r="BY8" s="41" t="n"/>
-      <c r="BZ8" s="41" t="n"/>
-      <c r="CA8" s="41" t="n"/>
-      <c r="CB8" s="41" t="n"/>
-      <c r="CC8" s="41" t="n"/>
-      <c r="CD8" s="41" t="n"/>
-      <c r="CE8" s="41" t="n"/>
-      <c r="CF8" s="41" t="n"/>
-      <c r="CG8" s="41" t="n"/>
-      <c r="CH8" s="41" t="n"/>
-      <c r="CI8" s="41" t="n"/>
-      <c r="CJ8" s="41" t="n"/>
-      <c r="CK8" s="41" t="n"/>
-      <c r="CL8" s="41" t="n"/>
-      <c r="CM8" s="41" t="n"/>
-      <c r="CN8" s="41" t="n"/>
-      <c r="CO8" s="41" t="n"/>
-      <c r="CP8" s="41" t="n"/>
-      <c r="CQ8" s="41" t="n"/>
-      <c r="CR8" s="41" t="n"/>
-      <c r="CS8" s="41" t="n"/>
-      <c r="CT8" s="41" t="n"/>
-      <c r="CU8" s="41" t="n"/>
-      <c r="CV8" s="41" t="n"/>
-      <c r="CW8" s="41" t="n"/>
-      <c r="CX8" s="41" t="n"/>
-      <c r="CY8" s="41" t="n"/>
-      <c r="CZ8" s="41" t="n"/>
-      <c r="DA8" s="41" t="n"/>
-      <c r="DB8" s="41" t="n"/>
-      <c r="DC8" s="41" t="n"/>
-      <c r="DD8" s="41" t="n"/>
-      <c r="DE8" s="41" t="n"/>
-      <c r="DF8" s="41" t="n"/>
-      <c r="DG8" s="41" t="n"/>
-      <c r="DH8" s="41" t="n"/>
-      <c r="DI8" s="41" t="n"/>
-      <c r="DJ8" s="41" t="n"/>
-      <c r="DK8" s="41" t="n"/>
-      <c r="DL8" s="41" t="n"/>
-      <c r="DM8" s="41" t="n"/>
-      <c r="DN8" s="41" t="n"/>
-      <c r="DO8" s="41" t="n"/>
-      <c r="DP8" s="41" t="n"/>
-      <c r="DQ8" s="41" t="n"/>
-      <c r="DR8" s="41" t="n"/>
-      <c r="DS8" s="41" t="n"/>
-      <c r="DT8" s="41" t="n"/>
-      <c r="DU8" s="41" t="n"/>
-      <c r="DV8" s="41" t="n"/>
-      <c r="DW8" s="41" t="n"/>
-      <c r="DX8" s="41" t="n"/>
-      <c r="DY8" s="41" t="n"/>
-      <c r="DZ8" s="41" t="n"/>
-      <c r="EA8" s="41" t="n"/>
-      <c r="EB8" s="41" t="n"/>
-      <c r="EC8" s="41" t="n"/>
-      <c r="ED8" s="41" t="n"/>
-      <c r="EE8" s="41" t="n"/>
-      <c r="EF8" s="41" t="n"/>
-      <c r="EG8" s="41" t="n"/>
-      <c r="EH8" s="41" t="n"/>
-      <c r="EI8" s="41" t="n"/>
-      <c r="EJ8" s="41" t="n"/>
-      <c r="EK8" s="41" t="n"/>
-      <c r="EL8" s="41" t="n"/>
-      <c r="EM8" s="41" t="n"/>
-      <c r="EN8" s="41" t="n"/>
-      <c r="EO8" s="41" t="n"/>
-      <c r="EP8" s="41" t="n"/>
-      <c r="EQ8" s="41" t="n"/>
-      <c r="ER8" s="41" t="n"/>
-      <c r="ES8" s="41" t="n"/>
-      <c r="ET8" s="41" t="n"/>
-      <c r="EU8" s="41" t="n"/>
-      <c r="EV8" s="41" t="n"/>
-      <c r="EW8" s="41" t="n"/>
-      <c r="EX8" s="41" t="n"/>
-      <c r="EY8" s="41" t="n"/>
-      <c r="EZ8" s="41" t="n"/>
-      <c r="FA8" s="41" t="n"/>
-      <c r="FB8" s="41" t="n"/>
-      <c r="FC8" s="41" t="n"/>
-      <c r="FD8" s="41" t="n"/>
-      <c r="FE8" s="41" t="n"/>
-      <c r="FF8" s="41" t="n"/>
-      <c r="FG8" s="41" t="n"/>
-      <c r="FH8" s="41" t="n"/>
-      <c r="FI8" s="41" t="n"/>
-      <c r="FJ8" s="41" t="n"/>
-    </row>
-    <row r="9" ht="13.8" customHeight="1" s="42">
-      <c r="A9" s="41" t="n"/>
-      <c r="B9" s="41" t="n"/>
-      <c r="C9" s="41" t="n"/>
-      <c r="D9" s="41" t="n"/>
-      <c r="E9" s="41" t="n"/>
-      <c r="F9" s="41" t="n"/>
-      <c r="H9" s="41" t="n"/>
-      <c r="I9" s="41" t="n"/>
-      <c r="J9" s="41" t="n"/>
-      <c r="K9" s="41" t="n"/>
-      <c r="L9" s="41" t="n"/>
-      <c r="M9" s="41" t="n"/>
-      <c r="N9" s="41" t="n"/>
-      <c r="O9" s="41" t="n"/>
-      <c r="P9" s="41" t="n"/>
-      <c r="Q9" s="41" t="n"/>
-      <c r="R9" s="41" t="n"/>
-      <c r="S9" s="41" t="n"/>
-      <c r="T9" s="41" t="n"/>
-      <c r="U9" s="41" t="n"/>
-      <c r="V9" s="41" t="n"/>
-      <c r="W9" s="41" t="n"/>
-      <c r="X9" s="41" t="n"/>
-      <c r="Y9" s="41" t="n"/>
-      <c r="Z9" s="41" t="n"/>
-      <c r="AA9" s="41" t="n"/>
-      <c r="AB9" s="41" t="n"/>
-      <c r="AC9" s="41" t="n"/>
-      <c r="AD9" s="41" t="n"/>
-      <c r="AE9" s="41" t="n"/>
-      <c r="AF9" s="41" t="n"/>
-      <c r="AG9" s="41" t="n"/>
-      <c r="AH9" s="41" t="n"/>
-      <c r="AI9" s="41" t="n"/>
-      <c r="AJ9" s="41" t="n"/>
-      <c r="AK9" s="41" t="n"/>
-      <c r="AL9" s="41" t="n"/>
-      <c r="AM9" s="41" t="n"/>
-      <c r="AN9" s="41" t="n"/>
-      <c r="AO9" s="41" t="n"/>
-      <c r="AP9" s="41" t="n"/>
-      <c r="AQ9" s="41" t="n"/>
-      <c r="AR9" s="41" t="n"/>
-      <c r="AS9" s="41" t="n"/>
-      <c r="AT9" s="41" t="n"/>
-      <c r="AU9" s="41" t="n"/>
-      <c r="AV9" s="41" t="n"/>
-      <c r="AW9" s="41" t="n"/>
-      <c r="AX9" s="41" t="n"/>
-      <c r="AY9" s="41" t="n"/>
-      <c r="AZ9" s="41" t="n"/>
-      <c r="BA9" s="41" t="n"/>
-      <c r="BB9" s="41" t="n"/>
-      <c r="BC9" s="41" t="n"/>
-      <c r="BD9" s="41" t="n"/>
-      <c r="BE9" s="41" t="n"/>
-      <c r="BF9" s="41" t="n"/>
-      <c r="BG9" s="41" t="n"/>
-      <c r="BH9" s="41" t="n"/>
-      <c r="BI9" s="41" t="n"/>
-      <c r="BJ9" s="41" t="n"/>
-      <c r="BK9" s="41" t="n"/>
-      <c r="BL9" s="41" t="n"/>
-      <c r="BM9" s="41" t="n"/>
-      <c r="BN9" s="41" t="n"/>
-      <c r="BO9" s="41" t="n"/>
-      <c r="BP9" s="41" t="n"/>
-      <c r="BQ9" s="41" t="n"/>
-      <c r="BR9" s="41" t="n"/>
-      <c r="BS9" s="41" t="n"/>
-      <c r="BT9" s="41" t="n"/>
-      <c r="BU9" s="41" t="n"/>
-      <c r="BV9" s="41" t="n"/>
-      <c r="BW9" s="41" t="n"/>
-      <c r="BX9" s="41" t="n"/>
-      <c r="BY9" s="41" t="n"/>
-      <c r="BZ9" s="41" t="n"/>
-      <c r="CA9" s="41" t="n"/>
-      <c r="CB9" s="41" t="n"/>
-      <c r="CC9" s="41" t="n"/>
-      <c r="CD9" s="41" t="n"/>
-      <c r="CE9" s="41" t="n"/>
-      <c r="CF9" s="41" t="n"/>
-      <c r="CG9" s="41" t="n"/>
-      <c r="CH9" s="41" t="n"/>
-      <c r="CI9" s="41" t="n"/>
-      <c r="CJ9" s="41" t="n"/>
-      <c r="CK9" s="41" t="n"/>
-      <c r="CL9" s="41" t="n"/>
-      <c r="CM9" s="41" t="n"/>
-      <c r="CN9" s="41" t="n"/>
-      <c r="CO9" s="41" t="n"/>
-      <c r="CP9" s="41" t="n"/>
-      <c r="CQ9" s="41" t="n"/>
-      <c r="CR9" s="41" t="n"/>
-      <c r="CS9" s="41" t="n"/>
-      <c r="CT9" s="41" t="n"/>
-      <c r="CU9" s="41" t="n"/>
-      <c r="CV9" s="41" t="n"/>
-      <c r="CW9" s="41" t="n"/>
-      <c r="CX9" s="41" t="n"/>
-      <c r="CY9" s="41" t="n"/>
-      <c r="CZ9" s="41" t="n"/>
-      <c r="DA9" s="41" t="n"/>
-      <c r="DB9" s="41" t="n"/>
-      <c r="DC9" s="41" t="n"/>
-      <c r="DD9" s="41" t="n"/>
-      <c r="DE9" s="41" t="n"/>
-      <c r="DF9" s="41" t="n"/>
-      <c r="DG9" s="41" t="n"/>
-      <c r="DH9" s="41" t="n"/>
-      <c r="DI9" s="41" t="n"/>
-      <c r="DJ9" s="41" t="n"/>
-      <c r="DK9" s="41" t="n"/>
-      <c r="DL9" s="41" t="n"/>
-      <c r="DM9" s="41" t="n"/>
-      <c r="DN9" s="41" t="n"/>
-      <c r="DO9" s="41" t="n"/>
-      <c r="DP9" s="41" t="n"/>
-      <c r="DQ9" s="41" t="n"/>
-      <c r="DR9" s="41" t="n"/>
-      <c r="DS9" s="41" t="n"/>
-      <c r="DT9" s="41" t="n"/>
-      <c r="DU9" s="41" t="n"/>
-      <c r="DV9" s="41" t="n"/>
-      <c r="DW9" s="41" t="n"/>
-      <c r="DX9" s="41" t="n"/>
-      <c r="DY9" s="41" t="n"/>
-      <c r="DZ9" s="41" t="n"/>
-      <c r="EA9" s="41" t="n"/>
-      <c r="EB9" s="41" t="n"/>
-      <c r="EC9" s="41" t="n"/>
-      <c r="ED9" s="41" t="n"/>
-      <c r="EE9" s="41" t="n"/>
-      <c r="EF9" s="41" t="n"/>
-      <c r="EG9" s="41" t="n"/>
-      <c r="EH9" s="41" t="n"/>
-      <c r="EI9" s="41" t="n"/>
-      <c r="EJ9" s="41" t="n"/>
-      <c r="EK9" s="41" t="n"/>
-      <c r="EL9" s="41" t="n"/>
-      <c r="EM9" s="41" t="n"/>
-      <c r="EN9" s="41" t="n"/>
-      <c r="EO9" s="41" t="n"/>
-      <c r="EP9" s="41" t="n"/>
-      <c r="EQ9" s="41" t="n"/>
-      <c r="ER9" s="41" t="n"/>
-      <c r="ES9" s="41" t="n"/>
-      <c r="ET9" s="41" t="n"/>
-      <c r="EU9" s="41" t="n"/>
-      <c r="EV9" s="41" t="n"/>
-      <c r="EW9" s="41" t="n"/>
-      <c r="EX9" s="41" t="n"/>
-      <c r="EY9" s="41" t="n"/>
-      <c r="EZ9" s="41" t="n"/>
-      <c r="FA9" s="41" t="n"/>
-      <c r="FB9" s="41" t="n"/>
-      <c r="FC9" s="41" t="n"/>
-      <c r="FD9" s="41" t="n"/>
-      <c r="FE9" s="41" t="n"/>
-      <c r="FF9" s="41" t="n"/>
-      <c r="FG9" s="41" t="n"/>
-      <c r="FH9" s="41" t="n"/>
-      <c r="FI9" s="41" t="n"/>
-      <c r="FJ9" s="41" t="n"/>
-    </row>
-    <row r="10" ht="13.8" customHeight="1" s="42">
-      <c r="A10" s="41" t="n"/>
-      <c r="B10" s="41" t="n"/>
-      <c r="C10" s="41" t="n"/>
-      <c r="D10" s="41" t="n"/>
-      <c r="E10" s="41" t="n"/>
-      <c r="F10" s="41" t="n"/>
-      <c r="H10" s="41" t="n"/>
-      <c r="I10" s="41" t="n"/>
-      <c r="J10" s="41" t="n"/>
-      <c r="K10" s="41" t="n"/>
-      <c r="L10" s="41" t="n"/>
-      <c r="M10" s="41" t="n"/>
-      <c r="N10" s="41" t="n"/>
-      <c r="O10" s="41" t="n"/>
-      <c r="P10" s="41" t="n"/>
-      <c r="Q10" s="41" t="n"/>
-      <c r="R10" s="41" t="n"/>
-      <c r="S10" s="41" t="n"/>
-      <c r="T10" s="41" t="n"/>
-      <c r="U10" s="41" t="n"/>
-      <c r="V10" s="41" t="n"/>
-      <c r="W10" s="41" t="n"/>
-      <c r="X10" s="41" t="n"/>
-      <c r="Y10" s="41" t="n"/>
-      <c r="Z10" s="41" t="n"/>
-      <c r="AA10" s="41" t="n"/>
-      <c r="AB10" s="41" t="n"/>
-      <c r="AC10" s="41" t="n"/>
-      <c r="AD10" s="41" t="n"/>
-      <c r="AE10" s="41" t="n"/>
-      <c r="AF10" s="41" t="n"/>
-      <c r="AG10" s="41" t="n"/>
-      <c r="AH10" s="41" t="n"/>
-      <c r="AI10" s="41" t="n"/>
-      <c r="AJ10" s="41" t="n"/>
-      <c r="AK10" s="41" t="n"/>
-      <c r="AL10" s="41" t="n"/>
-      <c r="AM10" s="41" t="n"/>
-      <c r="AN10" s="41" t="n"/>
-      <c r="AO10" s="41" t="n"/>
-      <c r="AP10" s="41" t="n"/>
-      <c r="AQ10" s="41" t="n"/>
-      <c r="AR10" s="41" t="n"/>
-      <c r="AS10" s="41" t="n"/>
-      <c r="AT10" s="41" t="n"/>
-      <c r="AU10" s="41" t="n"/>
-      <c r="AV10" s="41" t="n"/>
-      <c r="AW10" s="41" t="n"/>
-      <c r="AX10" s="41" t="n"/>
-      <c r="AY10" s="41" t="n"/>
-      <c r="AZ10" s="41" t="n"/>
-      <c r="BA10" s="41" t="n"/>
-      <c r="BB10" s="41" t="n"/>
-      <c r="BC10" s="41" t="n"/>
-      <c r="BD10" s="41" t="n"/>
-      <c r="BE10" s="41" t="n"/>
-      <c r="BF10" s="41" t="n"/>
-      <c r="BG10" s="41" t="n"/>
-      <c r="BH10" s="41" t="n"/>
-      <c r="BI10" s="41" t="n"/>
-      <c r="BJ10" s="41" t="n"/>
-      <c r="BK10" s="41" t="n"/>
-      <c r="BL10" s="41" t="n"/>
-      <c r="BM10" s="41" t="n"/>
-      <c r="BN10" s="41" t="n"/>
-      <c r="BO10" s="41" t="n"/>
-      <c r="BP10" s="41" t="n"/>
-      <c r="BQ10" s="41" t="n"/>
-      <c r="BR10" s="41" t="n"/>
-      <c r="BS10" s="41" t="n"/>
-      <c r="BT10" s="41" t="n"/>
-      <c r="BU10" s="41" t="n"/>
-      <c r="BV10" s="41" t="n"/>
-      <c r="BW10" s="41" t="n"/>
-      <c r="BX10" s="41" t="n"/>
-      <c r="BY10" s="41" t="n"/>
-      <c r="BZ10" s="41" t="n"/>
-      <c r="CA10" s="41" t="n"/>
-      <c r="CB10" s="41" t="n"/>
-      <c r="CC10" s="41" t="n"/>
-      <c r="CD10" s="41" t="n"/>
-      <c r="CE10" s="41" t="n"/>
-      <c r="CF10" s="41" t="n"/>
-      <c r="CG10" s="41" t="n"/>
-      <c r="CH10" s="41" t="n"/>
-      <c r="CI10" s="41" t="n"/>
-      <c r="CJ10" s="41" t="n"/>
-      <c r="CK10" s="41" t="n"/>
-      <c r="CL10" s="41" t="n"/>
-      <c r="CM10" s="41" t="n"/>
-      <c r="CN10" s="41" t="n"/>
-      <c r="CO10" s="41" t="n"/>
-      <c r="CP10" s="41" t="n"/>
-      <c r="CQ10" s="41" t="n"/>
-      <c r="CR10" s="41" t="n"/>
-      <c r="CS10" s="41" t="n"/>
-      <c r="CT10" s="41" t="n"/>
-      <c r="CU10" s="41" t="n"/>
-      <c r="CV10" s="41" t="n"/>
-      <c r="CW10" s="41" t="n"/>
-      <c r="CX10" s="41" t="n"/>
-      <c r="CY10" s="41" t="n"/>
-      <c r="CZ10" s="41" t="n"/>
-      <c r="DA10" s="41" t="n"/>
-      <c r="DB10" s="41" t="n"/>
-      <c r="DC10" s="41" t="n"/>
-      <c r="DD10" s="41" t="n"/>
-      <c r="DE10" s="41" t="n"/>
-      <c r="DF10" s="41" t="n"/>
-      <c r="DG10" s="41" t="n"/>
-      <c r="DH10" s="41" t="n"/>
-      <c r="DI10" s="41" t="n"/>
-      <c r="DJ10" s="41" t="n"/>
-      <c r="DK10" s="41" t="n"/>
-      <c r="DL10" s="41" t="n"/>
-      <c r="DM10" s="41" t="n"/>
-      <c r="DN10" s="41" t="n"/>
-      <c r="DO10" s="41" t="n"/>
-      <c r="DP10" s="41" t="n"/>
-      <c r="DQ10" s="41" t="n"/>
-      <c r="DR10" s="41" t="n"/>
-      <c r="DS10" s="41" t="n"/>
-      <c r="DT10" s="41" t="n"/>
-      <c r="DU10" s="41" t="n"/>
-      <c r="DV10" s="41" t="n"/>
-      <c r="DW10" s="41" t="n"/>
-      <c r="DX10" s="41" t="n"/>
-      <c r="DY10" s="41" t="n"/>
-      <c r="DZ10" s="41" t="n"/>
-      <c r="EA10" s="41" t="n"/>
-      <c r="EB10" s="41" t="n"/>
-      <c r="EC10" s="41" t="n"/>
-      <c r="ED10" s="41" t="n"/>
-      <c r="EE10" s="41" t="n"/>
-      <c r="EF10" s="41" t="n"/>
-      <c r="EG10" s="41" t="n"/>
-      <c r="EH10" s="41" t="n"/>
-      <c r="EI10" s="41" t="n"/>
-      <c r="EJ10" s="41" t="n"/>
-      <c r="EK10" s="41" t="n"/>
-      <c r="EL10" s="41" t="n"/>
-      <c r="EM10" s="41" t="n"/>
-      <c r="EN10" s="41" t="n"/>
-      <c r="EO10" s="41" t="n"/>
-      <c r="EP10" s="41" t="n"/>
-      <c r="EQ10" s="41" t="n"/>
-      <c r="ER10" s="41" t="n"/>
-      <c r="ES10" s="41" t="n"/>
-      <c r="ET10" s="41" t="n"/>
-      <c r="EU10" s="41" t="n"/>
-      <c r="EV10" s="41" t="n"/>
-      <c r="EW10" s="41" t="n"/>
-      <c r="EX10" s="41" t="n"/>
-      <c r="EY10" s="41" t="n"/>
-      <c r="EZ10" s="41" t="n"/>
-      <c r="FA10" s="41" t="n"/>
-      <c r="FB10" s="41" t="n"/>
-      <c r="FC10" s="41" t="n"/>
-      <c r="FD10" s="41" t="n"/>
-      <c r="FE10" s="41" t="n"/>
-      <c r="FF10" s="41" t="n"/>
-      <c r="FG10" s="41" t="n"/>
-      <c r="FH10" s="41" t="n"/>
-      <c r="FI10" s="41" t="n"/>
-      <c r="FJ10" s="41" t="n"/>
-    </row>
-    <row r="11" ht="13.8" customHeight="1" s="42">
-      <c r="A11" s="41" t="n"/>
-      <c r="B11" s="41" t="n"/>
-      <c r="C11" s="41" t="n"/>
-      <c r="D11" s="41" t="n"/>
-      <c r="E11" s="41" t="n"/>
-      <c r="F11" s="41" t="n"/>
-      <c r="H11" s="41" t="n"/>
-      <c r="I11" s="41" t="n"/>
-      <c r="J11" s="41" t="n"/>
-      <c r="K11" s="41" t="n"/>
-      <c r="L11" s="41" t="n"/>
-      <c r="M11" s="41" t="n"/>
-      <c r="N11" s="41" t="n"/>
-      <c r="O11" s="41" t="n"/>
-      <c r="P11" s="41" t="n"/>
-      <c r="Q11" s="41" t="n"/>
-      <c r="R11" s="41" t="n"/>
-      <c r="S11" s="41" t="n"/>
-      <c r="T11" s="41" t="n"/>
-      <c r="U11" s="41" t="n"/>
-      <c r="V11" s="41" t="n"/>
-      <c r="W11" s="41" t="n"/>
-      <c r="X11" s="41" t="n"/>
-      <c r="Y11" s="41" t="n"/>
-      <c r="Z11" s="41" t="n"/>
-      <c r="AA11" s="41" t="n"/>
-      <c r="AB11" s="41" t="n"/>
-      <c r="AC11" s="41" t="n"/>
-      <c r="AD11" s="41" t="n"/>
-      <c r="AE11" s="41" t="n"/>
-      <c r="AF11" s="41" t="n"/>
-      <c r="AG11" s="41" t="n"/>
-      <c r="AH11" s="41" t="n"/>
-      <c r="AI11" s="41" t="n"/>
-      <c r="AJ11" s="41" t="n"/>
-      <c r="AK11" s="41" t="n"/>
-      <c r="AL11" s="41" t="n"/>
-      <c r="AM11" s="41" t="n"/>
-      <c r="AN11" s="41" t="n"/>
-      <c r="AO11" s="41" t="n"/>
-      <c r="AP11" s="41" t="n"/>
-      <c r="AQ11" s="41" t="n"/>
-      <c r="AR11" s="41" t="n"/>
-      <c r="AS11" s="41" t="n"/>
-      <c r="AT11" s="41" t="n"/>
-      <c r="AU11" s="41" t="n"/>
-      <c r="AV11" s="41" t="n"/>
-      <c r="AW11" s="41" t="n"/>
-      <c r="AX11" s="41" t="n"/>
-      <c r="AY11" s="41" t="n"/>
-      <c r="AZ11" s="41" t="n"/>
-      <c r="BA11" s="41" t="n"/>
-      <c r="BB11" s="41" t="n"/>
-      <c r="BC11" s="41" t="n"/>
-      <c r="BD11" s="41" t="n"/>
-      <c r="BE11" s="41" t="n"/>
-      <c r="BF11" s="41" t="n"/>
-      <c r="BG11" s="41" t="n"/>
-      <c r="BH11" s="41" t="n"/>
-      <c r="BI11" s="41" t="n"/>
-      <c r="BJ11" s="41" t="n"/>
-      <c r="BK11" s="41" t="n"/>
-      <c r="BL11" s="41" t="n"/>
-      <c r="BM11" s="41" t="n"/>
-      <c r="BN11" s="41" t="n"/>
-      <c r="BO11" s="41" t="n"/>
-      <c r="BP11" s="41" t="n"/>
-      <c r="BQ11" s="41" t="n"/>
-      <c r="BR11" s="41" t="n"/>
-      <c r="BS11" s="41" t="n"/>
-      <c r="BT11" s="41" t="n"/>
-      <c r="BU11" s="41" t="n"/>
-      <c r="BV11" s="41" t="n"/>
-      <c r="BW11" s="41" t="n"/>
-      <c r="BX11" s="41" t="n"/>
-      <c r="BY11" s="41" t="n"/>
-      <c r="BZ11" s="41" t="n"/>
-      <c r="CA11" s="41" t="n"/>
-      <c r="CB11" s="41" t="n"/>
-      <c r="CC11" s="41" t="n"/>
-      <c r="CD11" s="41" t="n"/>
-      <c r="CE11" s="41" t="n"/>
-      <c r="CF11" s="41" t="n"/>
-      <c r="CG11" s="41" t="n"/>
-      <c r="CH11" s="41" t="n"/>
-      <c r="CI11" s="41" t="n"/>
-      <c r="CJ11" s="41" t="n"/>
-      <c r="CK11" s="41" t="n"/>
-      <c r="CL11" s="41" t="n"/>
-      <c r="CM11" s="41" t="n"/>
-      <c r="CN11" s="41" t="n"/>
-      <c r="CO11" s="41" t="n"/>
-      <c r="CP11" s="41" t="n"/>
-      <c r="CQ11" s="41" t="n"/>
-      <c r="CR11" s="41" t="n"/>
-      <c r="CS11" s="41" t="n"/>
-      <c r="CT11" s="41" t="n"/>
-      <c r="CU11" s="41" t="n"/>
-      <c r="CV11" s="41" t="n"/>
-      <c r="CW11" s="41" t="n"/>
-      <c r="CX11" s="41" t="n"/>
-      <c r="CY11" s="41" t="n"/>
-      <c r="CZ11" s="41" t="n"/>
-      <c r="DA11" s="41" t="n"/>
-      <c r="DB11" s="41" t="n"/>
-      <c r="DC11" s="41" t="n"/>
-      <c r="DD11" s="41" t="n"/>
-      <c r="DE11" s="41" t="n"/>
-      <c r="DF11" s="41" t="n"/>
-      <c r="DG11" s="41" t="n"/>
-      <c r="DH11" s="41" t="n"/>
-      <c r="DI11" s="41" t="n"/>
-      <c r="DJ11" s="41" t="n"/>
-      <c r="DK11" s="41" t="n"/>
-      <c r="DL11" s="41" t="n"/>
-      <c r="DM11" s="41" t="n"/>
-      <c r="DN11" s="41" t="n"/>
-      <c r="DO11" s="41" t="n"/>
-      <c r="DP11" s="41" t="n"/>
-      <c r="DQ11" s="41" t="n"/>
-      <c r="DR11" s="41" t="n"/>
-      <c r="DS11" s="41" t="n"/>
-      <c r="DT11" s="41" t="n"/>
-      <c r="DU11" s="41" t="n"/>
-      <c r="DV11" s="41" t="n"/>
-      <c r="DW11" s="41" t="n"/>
-      <c r="DX11" s="41" t="n"/>
-      <c r="DY11" s="41" t="n"/>
-      <c r="DZ11" s="41" t="n"/>
-      <c r="EA11" s="41" t="n"/>
-      <c r="EB11" s="41" t="n"/>
-      <c r="EC11" s="41" t="n"/>
-      <c r="ED11" s="41" t="n"/>
-      <c r="EE11" s="41" t="n"/>
-      <c r="EF11" s="41" t="n"/>
-      <c r="EG11" s="41" t="n"/>
-      <c r="EH11" s="41" t="n"/>
-      <c r="EI11" s="41" t="n"/>
-      <c r="EJ11" s="41" t="n"/>
-      <c r="EK11" s="41" t="n"/>
-      <c r="EL11" s="41" t="n"/>
-      <c r="EM11" s="41" t="n"/>
-      <c r="EN11" s="41" t="n"/>
-      <c r="EO11" s="41" t="n"/>
-      <c r="EP11" s="41" t="n"/>
-      <c r="EQ11" s="41" t="n"/>
-      <c r="ER11" s="41" t="n"/>
-      <c r="ES11" s="41" t="n"/>
-      <c r="ET11" s="41" t="n"/>
-      <c r="EU11" s="41" t="n"/>
-      <c r="EV11" s="41" t="n"/>
-      <c r="EW11" s="41" t="n"/>
-      <c r="EX11" s="41" t="n"/>
-      <c r="EY11" s="41" t="n"/>
-      <c r="EZ11" s="41" t="n"/>
-      <c r="FA11" s="41" t="n"/>
-      <c r="FB11" s="41" t="n"/>
-      <c r="FC11" s="41" t="n"/>
-      <c r="FD11" s="41" t="n"/>
-      <c r="FE11" s="41" t="n"/>
-      <c r="FF11" s="41" t="n"/>
-      <c r="FG11" s="41" t="n"/>
-      <c r="FH11" s="41" t="n"/>
-      <c r="FI11" s="41" t="n"/>
-      <c r="FJ11" s="41" t="n"/>
-    </row>
-    <row r="12" ht="13.8" customHeight="1" s="42">
-      <c r="A12" s="41" t="n"/>
-      <c r="B12" s="41" t="n"/>
-      <c r="C12" s="41" t="n"/>
-      <c r="D12" s="41" t="n"/>
-      <c r="E12" s="41" t="n"/>
-      <c r="F12" s="41" t="n"/>
-      <c r="H12" s="41" t="n"/>
-      <c r="I12" s="41" t="n"/>
-      <c r="J12" s="41" t="n"/>
-      <c r="K12" s="41" t="n"/>
-      <c r="L12" s="41" t="n"/>
-      <c r="M12" s="41" t="n"/>
-      <c r="N12" s="41" t="n"/>
-      <c r="O12" s="41" t="n"/>
-      <c r="P12" s="41" t="n"/>
-      <c r="Q12" s="41" t="n"/>
-      <c r="R12" s="41" t="n"/>
-      <c r="S12" s="41" t="n"/>
-      <c r="T12" s="41" t="n"/>
-      <c r="U12" s="41" t="n"/>
-      <c r="V12" s="41" t="n"/>
-      <c r="W12" s="41" t="n"/>
-      <c r="X12" s="41" t="n"/>
-      <c r="Y12" s="41" t="n"/>
-      <c r="Z12" s="41" t="n"/>
-      <c r="AA12" s="41" t="n"/>
-      <c r="AB12" s="41" t="n"/>
-      <c r="AC12" s="41" t="n"/>
-      <c r="AD12" s="41" t="n"/>
-      <c r="AE12" s="41" t="n"/>
-      <c r="AF12" s="41" t="n"/>
-      <c r="AG12" s="41" t="n"/>
-      <c r="AH12" s="41" t="n"/>
-      <c r="AI12" s="41" t="n"/>
-      <c r="AJ12" s="41" t="n"/>
-      <c r="AK12" s="41" t="n"/>
-      <c r="AL12" s="41" t="n"/>
-      <c r="AM12" s="41" t="n"/>
-      <c r="AN12" s="41" t="n"/>
-      <c r="AO12" s="41" t="n"/>
-      <c r="AP12" s="41" t="n"/>
-      <c r="AQ12" s="41" t="n"/>
-      <c r="AR12" s="41" t="n"/>
-      <c r="AS12" s="41" t="n"/>
-      <c r="AT12" s="41" t="n"/>
-      <c r="AU12" s="41" t="n"/>
-      <c r="AV12" s="41" t="n"/>
-      <c r="AW12" s="41" t="n"/>
-      <c r="AX12" s="41" t="n"/>
-      <c r="AY12" s="41" t="n"/>
-      <c r="AZ12" s="41" t="n"/>
-      <c r="BA12" s="41" t="n"/>
-      <c r="BB12" s="41" t="n"/>
-      <c r="BC12" s="41" t="n"/>
-      <c r="BD12" s="41" t="n"/>
-      <c r="BE12" s="41" t="n"/>
-      <c r="BF12" s="41" t="n"/>
-      <c r="BG12" s="41" t="n"/>
-      <c r="BH12" s="41" t="n"/>
-      <c r="BI12" s="41" t="n"/>
-      <c r="BJ12" s="41" t="n"/>
-      <c r="BK12" s="41" t="n"/>
-      <c r="BL12" s="41" t="n"/>
-      <c r="BM12" s="41" t="n"/>
-      <c r="BN12" s="41" t="n"/>
-      <c r="BO12" s="41" t="n"/>
-      <c r="BP12" s="41" t="n"/>
-      <c r="BQ12" s="41" t="n"/>
-      <c r="BR12" s="41" t="n"/>
-      <c r="BS12" s="41" t="n"/>
-      <c r="BT12" s="41" t="n"/>
-      <c r="BU12" s="41" t="n"/>
-      <c r="BV12" s="41" t="n"/>
-      <c r="BW12" s="41" t="n"/>
-      <c r="BX12" s="41" t="n"/>
-      <c r="BY12" s="41" t="n"/>
-      <c r="BZ12" s="41" t="n"/>
-      <c r="CA12" s="41" t="n"/>
-      <c r="CB12" s="41" t="n"/>
-      <c r="CC12" s="41" t="n"/>
-      <c r="CD12" s="41" t="n"/>
-      <c r="CE12" s="41" t="n"/>
-      <c r="CF12" s="41" t="n"/>
-      <c r="CG12" s="41" t="n"/>
-      <c r="CH12" s="41" t="n"/>
-      <c r="CI12" s="41" t="n"/>
-      <c r="CJ12" s="41" t="n"/>
-      <c r="CK12" s="41" t="n"/>
-      <c r="CL12" s="41" t="n"/>
-      <c r="CM12" s="41" t="n"/>
-      <c r="CN12" s="41" t="n"/>
-      <c r="CO12" s="41" t="n"/>
-      <c r="CP12" s="41" t="n"/>
-      <c r="CQ12" s="41" t="n"/>
-      <c r="CR12" s="41" t="n"/>
-      <c r="CS12" s="41" t="n"/>
-      <c r="CT12" s="41" t="n"/>
-      <c r="CU12" s="41" t="n"/>
-      <c r="CV12" s="41" t="n"/>
-      <c r="CW12" s="41" t="n"/>
-      <c r="CX12" s="41" t="n"/>
-      <c r="CY12" s="41" t="n"/>
-      <c r="CZ12" s="41" t="n"/>
-      <c r="DA12" s="41" t="n"/>
-      <c r="DB12" s="41" t="n"/>
-      <c r="DC12" s="41" t="n"/>
-      <c r="DD12" s="41" t="n"/>
-      <c r="DE12" s="41" t="n"/>
-      <c r="DF12" s="41" t="n"/>
-      <c r="DG12" s="41" t="n"/>
-      <c r="DH12" s="41" t="n"/>
-      <c r="DI12" s="41" t="n"/>
-      <c r="DJ12" s="41" t="n"/>
-      <c r="DK12" s="41" t="n"/>
-      <c r="DL12" s="41" t="n"/>
-      <c r="DM12" s="41" t="n"/>
-      <c r="DN12" s="41" t="n"/>
-      <c r="DO12" s="41" t="n"/>
-      <c r="DP12" s="41" t="n"/>
-      <c r="DQ12" s="41" t="n"/>
-      <c r="DR12" s="41" t="n"/>
-      <c r="DS12" s="41" t="n"/>
-      <c r="DT12" s="41" t="n"/>
-      <c r="DU12" s="41" t="n"/>
-      <c r="DV12" s="41" t="n"/>
-      <c r="DW12" s="41" t="n"/>
-      <c r="DX12" s="41" t="n"/>
-      <c r="DY12" s="41" t="n"/>
-      <c r="DZ12" s="41" t="n"/>
-      <c r="EA12" s="41" t="n"/>
-      <c r="EB12" s="41" t="n"/>
-      <c r="EC12" s="41" t="n"/>
-      <c r="ED12" s="41" t="n"/>
-      <c r="EE12" s="41" t="n"/>
-      <c r="EF12" s="41" t="n"/>
-      <c r="EG12" s="41" t="n"/>
-      <c r="EH12" s="41" t="n"/>
-      <c r="EI12" s="41" t="n"/>
-      <c r="EJ12" s="41" t="n"/>
-      <c r="EK12" s="41" t="n"/>
-      <c r="EL12" s="41" t="n"/>
-      <c r="EM12" s="41" t="n"/>
-      <c r="EN12" s="41" t="n"/>
-      <c r="EO12" s="41" t="n"/>
-      <c r="EP12" s="41" t="n"/>
-      <c r="EQ12" s="41" t="n"/>
-      <c r="ER12" s="41" t="n"/>
-      <c r="ES12" s="41" t="n"/>
-      <c r="ET12" s="41" t="n"/>
-      <c r="EU12" s="41" t="n"/>
-      <c r="EV12" s="41" t="n"/>
-      <c r="EW12" s="41" t="n"/>
-      <c r="EX12" s="41" t="n"/>
-      <c r="EY12" s="41" t="n"/>
-      <c r="EZ12" s="41" t="n"/>
-      <c r="FA12" s="41" t="n"/>
-      <c r="FB12" s="41" t="n"/>
-      <c r="FC12" s="41" t="n"/>
-      <c r="FD12" s="41" t="n"/>
-      <c r="FE12" s="41" t="n"/>
-      <c r="FF12" s="41" t="n"/>
-      <c r="FG12" s="41" t="n"/>
-      <c r="FH12" s="41" t="n"/>
-      <c r="FI12" s="41" t="n"/>
-      <c r="FJ12" s="41" t="n"/>
-    </row>
-    <row r="13" ht="13.8" customHeight="1" s="42">
-      <c r="A13" s="41" t="n"/>
-      <c r="B13" s="41" t="n"/>
-      <c r="C13" s="41" t="n"/>
-      <c r="D13" s="41" t="n"/>
-      <c r="E13" s="41" t="n"/>
-      <c r="F13" s="41" t="n"/>
-      <c r="H13" s="41" t="n"/>
-      <c r="I13" s="41" t="n"/>
-      <c r="J13" s="41" t="n"/>
-      <c r="K13" s="41" t="n"/>
-      <c r="L13" s="41" t="n"/>
-      <c r="M13" s="41" t="n"/>
-      <c r="N13" s="41" t="n"/>
-      <c r="O13" s="41" t="n"/>
-      <c r="P13" s="41" t="n"/>
-      <c r="Q13" s="41" t="n"/>
-      <c r="R13" s="41" t="n"/>
-      <c r="S13" s="41" t="n"/>
-      <c r="T13" s="41" t="n"/>
-      <c r="U13" s="41" t="n"/>
-      <c r="V13" s="41" t="n"/>
-      <c r="W13" s="41" t="n"/>
-      <c r="X13" s="41" t="n"/>
-      <c r="Y13" s="41" t="n"/>
-      <c r="Z13" s="41" t="n"/>
-      <c r="AA13" s="41" t="n"/>
-      <c r="AB13" s="41" t="n"/>
-      <c r="AC13" s="41" t="n"/>
-      <c r="AD13" s="41" t="n"/>
-      <c r="AE13" s="41" t="n"/>
-      <c r="AF13" s="41" t="n"/>
-      <c r="AG13" s="41" t="n"/>
-      <c r="AH13" s="41" t="n"/>
-      <c r="AI13" s="41" t="n"/>
-      <c r="AJ13" s="41" t="n"/>
-      <c r="AK13" s="41" t="n"/>
-      <c r="AL13" s="41" t="n"/>
-      <c r="AM13" s="41" t="n"/>
-      <c r="AN13" s="41" t="n"/>
-      <c r="AO13" s="41" t="n"/>
-      <c r="AP13" s="41" t="n"/>
-      <c r="AQ13" s="41" t="n"/>
-      <c r="AR13" s="41" t="n"/>
-      <c r="AS13" s="41" t="n"/>
-      <c r="AT13" s="41" t="n"/>
-      <c r="AU13" s="41" t="n"/>
-      <c r="AV13" s="41" t="n"/>
-      <c r="AW13" s="41" t="n"/>
-      <c r="AX13" s="41" t="n"/>
-      <c r="AY13" s="41" t="n"/>
-      <c r="AZ13" s="41" t="n"/>
-      <c r="BA13" s="41" t="n"/>
-      <c r="BB13" s="41" t="n"/>
-      <c r="BC13" s="41" t="n"/>
-      <c r="BD13" s="41" t="n"/>
-      <c r="BE13" s="41" t="n"/>
-      <c r="BF13" s="41" t="n"/>
-      <c r="BG13" s="41" t="n"/>
-      <c r="BH13" s="41" t="n"/>
-      <c r="BI13" s="41" t="n"/>
-      <c r="BJ13" s="41" t="n"/>
-      <c r="BK13" s="41" t="n"/>
-      <c r="BL13" s="41" t="n"/>
-      <c r="BM13" s="41" t="n"/>
-      <c r="BN13" s="41" t="n"/>
-      <c r="BO13" s="41" t="n"/>
-      <c r="BP13" s="41" t="n"/>
-      <c r="BQ13" s="41" t="n"/>
-      <c r="BR13" s="41" t="n"/>
-      <c r="BS13" s="41" t="n"/>
-      <c r="BT13" s="41" t="n"/>
-      <c r="BU13" s="41" t="n"/>
-      <c r="BV13" s="41" t="n"/>
-      <c r="BW13" s="41" t="n"/>
-      <c r="BX13" s="41" t="n"/>
-      <c r="BY13" s="41" t="n"/>
-      <c r="BZ13" s="41" t="n"/>
-      <c r="CA13" s="41" t="n"/>
-      <c r="CB13" s="41" t="n"/>
-      <c r="CC13" s="41" t="n"/>
-      <c r="CD13" s="41" t="n"/>
-      <c r="CE13" s="41" t="n"/>
-      <c r="CF13" s="41" t="n"/>
-      <c r="CG13" s="41" t="n"/>
-      <c r="CH13" s="41" t="n"/>
-      <c r="CI13" s="41" t="n"/>
-      <c r="CJ13" s="41" t="n"/>
-      <c r="CK13" s="41" t="n"/>
-      <c r="CL13" s="41" t="n"/>
-      <c r="CM13" s="41" t="n"/>
-      <c r="CN13" s="41" t="n"/>
-      <c r="CO13" s="41" t="n"/>
-      <c r="CP13" s="41" t="n"/>
-      <c r="CQ13" s="41" t="n"/>
-      <c r="CR13" s="41" t="n"/>
-      <c r="CS13" s="41" t="n"/>
-      <c r="CT13" s="41" t="n"/>
-      <c r="CU13" s="41" t="n"/>
-      <c r="CV13" s="41" t="n"/>
-      <c r="CW13" s="41" t="n"/>
-      <c r="CX13" s="41" t="n"/>
-      <c r="CY13" s="41" t="n"/>
-      <c r="CZ13" s="41" t="n"/>
-      <c r="DA13" s="41" t="n"/>
-      <c r="DB13" s="41" t="n"/>
-      <c r="DC13" s="41" t="n"/>
-      <c r="DD13" s="41" t="n"/>
-      <c r="DE13" s="41" t="n"/>
-      <c r="DF13" s="41" t="n"/>
-      <c r="DG13" s="41" t="n"/>
-      <c r="DH13" s="41" t="n"/>
-      <c r="DI13" s="41" t="n"/>
-      <c r="DJ13" s="41" t="n"/>
-      <c r="DK13" s="41" t="n"/>
-      <c r="DL13" s="41" t="n"/>
-      <c r="DM13" s="41" t="n"/>
-      <c r="DN13" s="41" t="n"/>
-      <c r="DO13" s="41" t="n"/>
-      <c r="DP13" s="41" t="n"/>
-      <c r="DQ13" s="41" t="n"/>
-      <c r="DR13" s="41" t="n"/>
-      <c r="DS13" s="41" t="n"/>
-      <c r="DT13" s="41" t="n"/>
-      <c r="DU13" s="41" t="n"/>
-      <c r="DV13" s="41" t="n"/>
-      <c r="DW13" s="41" t="n"/>
-      <c r="DX13" s="41" t="n"/>
-      <c r="DY13" s="41" t="n"/>
-      <c r="DZ13" s="41" t="n"/>
-      <c r="EA13" s="41" t="n"/>
-      <c r="EB13" s="41" t="n"/>
-      <c r="EC13" s="41" t="n"/>
-      <c r="ED13" s="41" t="n"/>
-      <c r="EE13" s="41" t="n"/>
-      <c r="EF13" s="41" t="n"/>
-      <c r="EG13" s="41" t="n"/>
-      <c r="EH13" s="41" t="n"/>
-      <c r="EI13" s="41" t="n"/>
-      <c r="EJ13" s="41" t="n"/>
-      <c r="EK13" s="41" t="n"/>
-      <c r="EL13" s="41" t="n"/>
-      <c r="EM13" s="41" t="n"/>
-      <c r="EN13" s="41" t="n"/>
-      <c r="EO13" s="41" t="n"/>
-      <c r="EP13" s="41" t="n"/>
-      <c r="EQ13" s="41" t="n"/>
-      <c r="ER13" s="41" t="n"/>
-      <c r="ES13" s="41" t="n"/>
-      <c r="ET13" s="41" t="n"/>
-      <c r="EU13" s="41" t="n"/>
-      <c r="EV13" s="41" t="n"/>
-      <c r="EW13" s="41" t="n"/>
-      <c r="EX13" s="41" t="n"/>
-      <c r="EY13" s="41" t="n"/>
-      <c r="EZ13" s="41" t="n"/>
-      <c r="FA13" s="41" t="n"/>
-      <c r="FB13" s="41" t="n"/>
-      <c r="FC13" s="41" t="n"/>
-      <c r="FD13" s="41" t="n"/>
-      <c r="FE13" s="41" t="n"/>
-      <c r="FF13" s="41" t="n"/>
-      <c r="FG13" s="41" t="n"/>
-      <c r="FH13" s="41" t="n"/>
-      <c r="FI13" s="41" t="n"/>
-      <c r="FJ13" s="41" t="n"/>
-    </row>
-    <row r="14" ht="13.8" customHeight="1" s="42">
-      <c r="A14" s="41" t="n"/>
-      <c r="B14" s="41" t="n"/>
-      <c r="C14" s="41" t="n"/>
-      <c r="D14" s="41" t="n"/>
-      <c r="E14" s="41" t="n"/>
-      <c r="F14" s="41" t="n"/>
-      <c r="H14" s="41" t="n"/>
-      <c r="I14" s="41" t="n"/>
-      <c r="J14" s="41" t="n"/>
-      <c r="K14" s="41" t="n"/>
-      <c r="L14" s="41" t="n"/>
-      <c r="M14" s="41" t="n"/>
-      <c r="N14" s="41" t="n"/>
-      <c r="O14" s="41" t="n"/>
-      <c r="P14" s="41" t="n"/>
-      <c r="Q14" s="41" t="n"/>
-      <c r="R14" s="41" t="n"/>
-      <c r="S14" s="41" t="n"/>
-      <c r="T14" s="41" t="n"/>
-      <c r="U14" s="41" t="n"/>
-      <c r="V14" s="41" t="n"/>
-      <c r="W14" s="41" t="n"/>
-      <c r="X14" s="41" t="n"/>
-      <c r="Y14" s="41" t="n"/>
-      <c r="Z14" s="41" t="n"/>
-      <c r="AA14" s="41" t="n"/>
-      <c r="AB14" s="41" t="n"/>
-      <c r="AC14" s="41" t="n"/>
-      <c r="AD14" s="41" t="n"/>
-      <c r="AE14" s="41" t="n"/>
-      <c r="AF14" s="41" t="n"/>
-      <c r="AG14" s="41" t="n"/>
-      <c r="AH14" s="41" t="n"/>
-      <c r="AI14" s="41" t="n"/>
-      <c r="AJ14" s="41" t="n"/>
-      <c r="AK14" s="41" t="n"/>
-      <c r="AL14" s="41" t="n"/>
-      <c r="AM14" s="41" t="n"/>
-      <c r="AN14" s="41" t="n"/>
-      <c r="AO14" s="41" t="n"/>
-      <c r="AP14" s="41" t="n"/>
-      <c r="AQ14" s="41" t="n"/>
-      <c r="AR14" s="41" t="n"/>
-      <c r="AS14" s="41" t="n"/>
-      <c r="AT14" s="41" t="n"/>
-      <c r="AU14" s="41" t="n"/>
-      <c r="AV14" s="41" t="n"/>
-      <c r="AW14" s="41" t="n"/>
-      <c r="AX14" s="41" t="n"/>
-      <c r="AY14" s="41" t="n"/>
-      <c r="AZ14" s="41" t="n"/>
-      <c r="BA14" s="41" t="n"/>
-      <c r="BB14" s="41" t="n"/>
-      <c r="BC14" s="41" t="n"/>
-      <c r="BD14" s="41" t="n"/>
-      <c r="BE14" s="41" t="n"/>
-      <c r="BF14" s="41" t="n"/>
-      <c r="BG14" s="41" t="n"/>
-      <c r="BH14" s="41" t="n"/>
-      <c r="BI14" s="41" t="n"/>
-      <c r="BJ14" s="41" t="n"/>
-      <c r="BK14" s="41" t="n"/>
-      <c r="BL14" s="41" t="n"/>
-      <c r="BM14" s="41" t="n"/>
-      <c r="BN14" s="41" t="n"/>
-      <c r="BO14" s="41" t="n"/>
-      <c r="BP14" s="41" t="n"/>
-      <c r="BQ14" s="41" t="n"/>
-      <c r="BR14" s="41" t="n"/>
-      <c r="BS14" s="41" t="n"/>
-      <c r="BT14" s="41" t="n"/>
-      <c r="BU14" s="41" t="n"/>
-      <c r="BV14" s="41" t="n"/>
-      <c r="BW14" s="41" t="n"/>
-      <c r="BX14" s="41" t="n"/>
-      <c r="BY14" s="41" t="n"/>
-      <c r="BZ14" s="41" t="n"/>
-      <c r="CA14" s="41" t="n"/>
-      <c r="CB14" s="41" t="n"/>
-      <c r="CC14" s="41" t="n"/>
-      <c r="CD14" s="41" t="n"/>
-      <c r="CE14" s="41" t="n"/>
-      <c r="CF14" s="41" t="n"/>
-      <c r="CG14" s="41" t="n"/>
-      <c r="CH14" s="41" t="n"/>
-      <c r="CI14" s="41" t="n"/>
-      <c r="CJ14" s="41" t="n"/>
-      <c r="CK14" s="41" t="n"/>
-      <c r="CL14" s="41" t="n"/>
-      <c r="CM14" s="41" t="n"/>
-      <c r="CN14" s="41" t="n"/>
-      <c r="CO14" s="41" t="n"/>
-      <c r="CP14" s="41" t="n"/>
-      <c r="CQ14" s="41" t="n"/>
-      <c r="CR14" s="41" t="n"/>
-      <c r="CS14" s="41" t="n"/>
-      <c r="CT14" s="41" t="n"/>
-      <c r="CU14" s="41" t="n"/>
-      <c r="CV14" s="41" t="n"/>
-      <c r="CW14" s="41" t="n"/>
-      <c r="CX14" s="41" t="n"/>
-      <c r="CY14" s="41" t="n"/>
-      <c r="CZ14" s="41" t="n"/>
-      <c r="DA14" s="41" t="n"/>
-      <c r="DB14" s="41" t="n"/>
-      <c r="DC14" s="41" t="n"/>
-      <c r="DD14" s="41" t="n"/>
-      <c r="DE14" s="41" t="n"/>
-      <c r="DF14" s="41" t="n"/>
-      <c r="DG14" s="41" t="n"/>
-      <c r="DH14" s="41" t="n"/>
-      <c r="DI14" s="41" t="n"/>
-      <c r="DJ14" s="41" t="n"/>
-      <c r="DK14" s="41" t="n"/>
-      <c r="DL14" s="41" t="n"/>
-      <c r="DM14" s="41" t="n"/>
-      <c r="DN14" s="41" t="n"/>
-      <c r="DO14" s="41" t="n"/>
-      <c r="DP14" s="41" t="n"/>
-      <c r="DQ14" s="41" t="n"/>
-      <c r="DR14" s="41" t="n"/>
-      <c r="DS14" s="41" t="n"/>
-      <c r="DT14" s="41" t="n"/>
-      <c r="DU14" s="41" t="n"/>
-      <c r="DV14" s="41" t="n"/>
-      <c r="DW14" s="41" t="n"/>
-      <c r="DX14" s="41" t="n"/>
-      <c r="DY14" s="41" t="n"/>
-      <c r="DZ14" s="41" t="n"/>
-      <c r="EA14" s="41" t="n"/>
-      <c r="EB14" s="41" t="n"/>
-      <c r="EC14" s="41" t="n"/>
-      <c r="ED14" s="41" t="n"/>
-      <c r="EE14" s="41" t="n"/>
-      <c r="EF14" s="41" t="n"/>
-      <c r="EG14" s="41" t="n"/>
-      <c r="EH14" s="41" t="n"/>
-      <c r="EI14" s="41" t="n"/>
-      <c r="EJ14" s="41" t="n"/>
-      <c r="EK14" s="41" t="n"/>
-      <c r="EL14" s="41" t="n"/>
-      <c r="EM14" s="41" t="n"/>
-      <c r="EN14" s="41" t="n"/>
-      <c r="EO14" s="41" t="n"/>
-      <c r="EP14" s="41" t="n"/>
-      <c r="EQ14" s="41" t="n"/>
-      <c r="ER14" s="41" t="n"/>
-      <c r="ES14" s="41" t="n"/>
-      <c r="ET14" s="41" t="n"/>
-      <c r="EU14" s="41" t="n"/>
-      <c r="EV14" s="41" t="n"/>
-      <c r="EW14" s="41" t="n"/>
-      <c r="EX14" s="41" t="n"/>
-      <c r="EY14" s="41" t="n"/>
-      <c r="EZ14" s="41" t="n"/>
-      <c r="FA14" s="41" t="n"/>
-      <c r="FB14" s="41" t="n"/>
-      <c r="FC14" s="41" t="n"/>
-      <c r="FD14" s="41" t="n"/>
-      <c r="FE14" s="41" t="n"/>
-      <c r="FF14" s="41" t="n"/>
-      <c r="FG14" s="41" t="n"/>
-      <c r="FH14" s="41" t="n"/>
-      <c r="FI14" s="41" t="n"/>
-      <c r="FJ14" s="41" t="n"/>
-    </row>
-    <row r="15" ht="13.8" customHeight="1" s="42">
-      <c r="A15" s="41" t="n"/>
-      <c r="B15" s="41" t="n"/>
-      <c r="C15" s="41" t="n"/>
-      <c r="D15" s="41" t="n"/>
-      <c r="E15" s="41" t="n"/>
-      <c r="F15" s="41" t="n"/>
-      <c r="H15" s="41" t="n"/>
-      <c r="I15" s="41" t="n"/>
-      <c r="J15" s="41" t="n"/>
-      <c r="K15" s="41" t="n"/>
-      <c r="L15" s="41" t="n"/>
-      <c r="M15" s="41" t="n"/>
-      <c r="N15" s="41" t="n"/>
-      <c r="O15" s="41" t="n"/>
-      <c r="P15" s="41" t="n"/>
-      <c r="Q15" s="41" t="n"/>
-      <c r="R15" s="41" t="n"/>
-      <c r="S15" s="41" t="n"/>
-      <c r="T15" s="41" t="n"/>
-      <c r="U15" s="41" t="n"/>
-      <c r="V15" s="41" t="n"/>
-      <c r="W15" s="41" t="n"/>
-      <c r="X15" s="41" t="n"/>
-      <c r="Y15" s="41" t="n"/>
-      <c r="Z15" s="41" t="n"/>
-      <c r="AA15" s="41" t="n"/>
-      <c r="AB15" s="41" t="n"/>
-      <c r="AC15" s="41" t="n"/>
-      <c r="AD15" s="41" t="n"/>
-      <c r="AE15" s="41" t="n"/>
-      <c r="AF15" s="41" t="n"/>
-      <c r="AG15" s="41" t="n"/>
-      <c r="AH15" s="41" t="n"/>
-      <c r="AI15" s="41" t="n"/>
-      <c r="AJ15" s="41" t="n"/>
-      <c r="AK15" s="41" t="n"/>
-      <c r="AL15" s="41" t="n"/>
-      <c r="AM15" s="41" t="n"/>
-      <c r="AN15" s="41" t="n"/>
-      <c r="AO15" s="41" t="n"/>
-      <c r="AP15" s="41" t="n"/>
-      <c r="AQ15" s="41" t="n"/>
-      <c r="AR15" s="41" t="n"/>
-      <c r="AS15" s="41" t="n"/>
-      <c r="AT15" s="41" t="n"/>
-      <c r="AU15" s="41" t="n"/>
-      <c r="AV15" s="41" t="n"/>
-      <c r="AW15" s="41" t="n"/>
-      <c r="AX15" s="41" t="n"/>
-      <c r="AY15" s="41" t="n"/>
-      <c r="AZ15" s="41" t="n"/>
-      <c r="BA15" s="41" t="n"/>
-      <c r="BB15" s="41" t="n"/>
-      <c r="BC15" s="41" t="n"/>
-      <c r="BD15" s="41" t="n"/>
-      <c r="BE15" s="41" t="n"/>
-      <c r="BF15" s="41" t="n"/>
-      <c r="BG15" s="41" t="n"/>
-      <c r="BH15" s="41" t="n"/>
-      <c r="BI15" s="41" t="n"/>
-      <c r="BJ15" s="41" t="n"/>
-      <c r="BK15" s="41" t="n"/>
-      <c r="BL15" s="41" t="n"/>
-      <c r="BM15" s="41" t="n"/>
-      <c r="BN15" s="41" t="n"/>
-      <c r="BO15" s="41" t="n"/>
-      <c r="BP15" s="41" t="n"/>
-      <c r="BQ15" s="41" t="n"/>
-      <c r="BR15" s="41" t="n"/>
-      <c r="BS15" s="41" t="n"/>
-      <c r="BT15" s="41" t="n"/>
-      <c r="BU15" s="41" t="n"/>
-      <c r="BV15" s="41" t="n"/>
-      <c r="BW15" s="41" t="n"/>
-      <c r="BX15" s="41" t="n"/>
-      <c r="BY15" s="41" t="n"/>
-      <c r="BZ15" s="41" t="n"/>
-      <c r="CA15" s="41" t="n"/>
-      <c r="CB15" s="41" t="n"/>
-      <c r="CC15" s="41" t="n"/>
-      <c r="CD15" s="41" t="n"/>
-      <c r="CE15" s="41" t="n"/>
-      <c r="CF15" s="41" t="n"/>
-      <c r="CG15" s="41" t="n"/>
-      <c r="CH15" s="41" t="n"/>
-      <c r="CI15" s="41" t="n"/>
-      <c r="CJ15" s="41" t="n"/>
-      <c r="CK15" s="41" t="n"/>
-      <c r="CL15" s="41" t="n"/>
-      <c r="CM15" s="41" t="n"/>
-      <c r="CN15" s="41" t="n"/>
-      <c r="CO15" s="41" t="n"/>
-      <c r="CP15" s="41" t="n"/>
-      <c r="CQ15" s="41" t="n"/>
-      <c r="CR15" s="41" t="n"/>
-      <c r="CS15" s="41" t="n"/>
-      <c r="CT15" s="41" t="n"/>
-      <c r="CU15" s="41" t="n"/>
-      <c r="CV15" s="41" t="n"/>
-      <c r="CW15" s="41" t="n"/>
-      <c r="CX15" s="41" t="n"/>
-      <c r="CY15" s="41" t="n"/>
-      <c r="CZ15" s="41" t="n"/>
-      <c r="DA15" s="41" t="n"/>
-      <c r="DB15" s="41" t="n"/>
-      <c r="DC15" s="41" t="n"/>
-      <c r="DD15" s="41" t="n"/>
-      <c r="DE15" s="41" t="n"/>
-      <c r="DF15" s="41" t="n"/>
-      <c r="DG15" s="41" t="n"/>
-      <c r="DH15" s="41" t="n"/>
-      <c r="DI15" s="41" t="n"/>
-      <c r="DJ15" s="41" t="n"/>
-      <c r="DK15" s="41" t="n"/>
-      <c r="DL15" s="41" t="n"/>
-      <c r="DM15" s="41" t="n"/>
-      <c r="DN15" s="41" t="n"/>
-      <c r="DO15" s="41" t="n"/>
-      <c r="DP15" s="41" t="n"/>
-      <c r="DQ15" s="41" t="n"/>
-      <c r="DR15" s="41" t="n"/>
-      <c r="DS15" s="41" t="n"/>
-      <c r="DT15" s="41" t="n"/>
-      <c r="DU15" s="41" t="n"/>
-      <c r="DV15" s="41" t="n"/>
-      <c r="DW15" s="41" t="n"/>
-      <c r="DX15" s="41" t="n"/>
-      <c r="DY15" s="41" t="n"/>
-      <c r="DZ15" s="41" t="n"/>
-      <c r="EA15" s="41" t="n"/>
-      <c r="EB15" s="41" t="n"/>
-      <c r="EC15" s="41" t="n"/>
-      <c r="ED15" s="41" t="n"/>
-      <c r="EE15" s="41" t="n"/>
-      <c r="EF15" s="41" t="n"/>
-      <c r="EG15" s="41" t="n"/>
-      <c r="EH15" s="41" t="n"/>
-      <c r="EI15" s="41" t="n"/>
-      <c r="EJ15" s="41" t="n"/>
-      <c r="EK15" s="41" t="n"/>
-      <c r="EL15" s="41" t="n"/>
-      <c r="EM15" s="41" t="n"/>
-      <c r="EN15" s="41" t="n"/>
-      <c r="EO15" s="41" t="n"/>
-      <c r="EP15" s="41" t="n"/>
-      <c r="EQ15" s="41" t="n"/>
-      <c r="ER15" s="41" t="n"/>
-      <c r="ES15" s="41" t="n"/>
-      <c r="ET15" s="41" t="n"/>
-      <c r="EU15" s="41" t="n"/>
-      <c r="EV15" s="41" t="n"/>
-      <c r="EW15" s="41" t="n"/>
-      <c r="EX15" s="41" t="n"/>
-      <c r="EY15" s="41" t="n"/>
-      <c r="EZ15" s="41" t="n"/>
-      <c r="FA15" s="41" t="n"/>
-      <c r="FB15" s="41" t="n"/>
-      <c r="FC15" s="41" t="n"/>
-      <c r="FD15" s="41" t="n"/>
-      <c r="FE15" s="41" t="n"/>
-      <c r="FF15" s="41" t="n"/>
-      <c r="FG15" s="41" t="n"/>
-      <c r="FH15" s="41" t="n"/>
-      <c r="FI15" s="41" t="n"/>
-      <c r="FJ15" s="41" t="n"/>
-    </row>
-    <row r="16" ht="13.8" customHeight="1" s="42">
-      <c r="A16" s="41" t="n"/>
-      <c r="B16" s="41" t="n"/>
-      <c r="C16" s="41" t="n"/>
-      <c r="D16" s="41" t="n"/>
-      <c r="E16" s="41" t="n"/>
-      <c r="F16" s="41" t="n"/>
-      <c r="H16" s="41" t="n"/>
-      <c r="I16" s="41" t="n"/>
-      <c r="J16" s="41" t="n"/>
-      <c r="K16" s="41" t="n"/>
-      <c r="L16" s="41" t="n"/>
-      <c r="M16" s="41" t="n"/>
-      <c r="N16" s="41" t="n"/>
-      <c r="O16" s="41" t="n"/>
-      <c r="P16" s="41" t="n"/>
-      <c r="Q16" s="41" t="n"/>
-      <c r="R16" s="41" t="n"/>
-      <c r="S16" s="41" t="n"/>
-      <c r="T16" s="41" t="n"/>
-      <c r="U16" s="41" t="n"/>
-      <c r="V16" s="41" t="n"/>
-      <c r="W16" s="41" t="n"/>
-      <c r="X16" s="41" t="n"/>
-      <c r="Y16" s="41" t="n"/>
-      <c r="Z16" s="41" t="n"/>
-      <c r="AA16" s="41" t="n"/>
-      <c r="AB16" s="41" t="n"/>
-      <c r="AC16" s="41" t="n"/>
-      <c r="AD16" s="41" t="n"/>
-      <c r="AE16" s="41" t="n"/>
-      <c r="AF16" s="41" t="n"/>
-      <c r="AG16" s="41" t="n"/>
-      <c r="AH16" s="41" t="n"/>
-      <c r="AI16" s="41" t="n"/>
-      <c r="AJ16" s="41" t="n"/>
-      <c r="AK16" s="41" t="n"/>
-      <c r="AL16" s="41" t="n"/>
-      <c r="AM16" s="41" t="n"/>
-      <c r="AN16" s="41" t="n"/>
-      <c r="AO16" s="41" t="n"/>
-      <c r="AP16" s="41" t="n"/>
-      <c r="AQ16" s="41" t="n"/>
-      <c r="AR16" s="41" t="n"/>
-      <c r="AS16" s="41" t="n"/>
-      <c r="AT16" s="41" t="n"/>
-      <c r="AU16" s="41" t="n"/>
-      <c r="AV16" s="41" t="n"/>
-      <c r="AW16" s="41" t="n"/>
-      <c r="AX16" s="41" t="n"/>
-      <c r="AY16" s="41" t="n"/>
-      <c r="AZ16" s="41" t="n"/>
-      <c r="BA16" s="41" t="n"/>
-      <c r="BB16" s="41" t="n"/>
-      <c r="BC16" s="41" t="n"/>
-      <c r="BD16" s="41" t="n"/>
-      <c r="BE16" s="41" t="n"/>
-      <c r="BF16" s="41" t="n"/>
-      <c r="BG16" s="41" t="n"/>
-      <c r="BH16" s="41" t="n"/>
-      <c r="BI16" s="41" t="n"/>
-      <c r="BJ16" s="41" t="n"/>
-      <c r="BK16" s="41" t="n"/>
-      <c r="BL16" s="41" t="n"/>
-      <c r="BM16" s="41" t="n"/>
-      <c r="BN16" s="41" t="n"/>
-      <c r="BO16" s="41" t="n"/>
-      <c r="BP16" s="41" t="n"/>
-      <c r="BQ16" s="41" t="n"/>
-      <c r="BR16" s="41" t="n"/>
-      <c r="BS16" s="41" t="n"/>
-      <c r="BT16" s="41" t="n"/>
-      <c r="BU16" s="41" t="n"/>
-      <c r="BV16" s="41" t="n"/>
-      <c r="BW16" s="41" t="n"/>
-      <c r="BX16" s="41" t="n"/>
-      <c r="BY16" s="41" t="n"/>
-      <c r="BZ16" s="41" t="n"/>
-      <c r="CA16" s="41" t="n"/>
-      <c r="CB16" s="41" t="n"/>
-      <c r="CC16" s="41" t="n"/>
-      <c r="CD16" s="41" t="n"/>
-      <c r="CE16" s="41" t="n"/>
-      <c r="CF16" s="41" t="n"/>
-      <c r="CG16" s="41" t="n"/>
-      <c r="CH16" s="41" t="n"/>
-      <c r="CI16" s="41" t="n"/>
-      <c r="CJ16" s="41" t="n"/>
-      <c r="CK16" s="41" t="n"/>
-      <c r="CL16" s="41" t="n"/>
-      <c r="CM16" s="41" t="n"/>
-      <c r="CN16" s="41" t="n"/>
-      <c r="CO16" s="41" t="n"/>
-      <c r="CP16" s="41" t="n"/>
-      <c r="CQ16" s="41" t="n"/>
-      <c r="CR16" s="41" t="n"/>
-      <c r="CS16" s="41" t="n"/>
-      <c r="CT16" s="41" t="n"/>
-      <c r="CU16" s="41" t="n"/>
-      <c r="CV16" s="41" t="n"/>
-      <c r="CW16" s="41" t="n"/>
-      <c r="CX16" s="41" t="n"/>
-      <c r="CY16" s="41" t="n"/>
-      <c r="CZ16" s="41" t="n"/>
-      <c r="DA16" s="41" t="n"/>
-      <c r="DB16" s="41" t="n"/>
-      <c r="DC16" s="41" t="n"/>
-      <c r="DD16" s="41" t="n"/>
-      <c r="DE16" s="41" t="n"/>
-      <c r="DF16" s="41" t="n"/>
-      <c r="DG16" s="41" t="n"/>
-      <c r="DH16" s="41" t="n"/>
-      <c r="DI16" s="41" t="n"/>
-      <c r="DJ16" s="41" t="n"/>
-      <c r="DK16" s="41" t="n"/>
-      <c r="DL16" s="41" t="n"/>
-      <c r="DM16" s="41" t="n"/>
-      <c r="DN16" s="41" t="n"/>
-      <c r="DO16" s="41" t="n"/>
-      <c r="DP16" s="41" t="n"/>
-      <c r="DQ16" s="41" t="n"/>
-      <c r="DR16" s="41" t="n"/>
-      <c r="DS16" s="41" t="n"/>
-      <c r="DT16" s="41" t="n"/>
-      <c r="DU16" s="41" t="n"/>
-      <c r="DV16" s="41" t="n"/>
-      <c r="DW16" s="41" t="n"/>
-      <c r="DX16" s="41" t="n"/>
-      <c r="DY16" s="41" t="n"/>
-      <c r="DZ16" s="41" t="n"/>
-      <c r="EA16" s="41" t="n"/>
-      <c r="EB16" s="41" t="n"/>
-      <c r="EC16" s="41" t="n"/>
-      <c r="ED16" s="41" t="n"/>
-      <c r="EE16" s="41" t="n"/>
-      <c r="EF16" s="41" t="n"/>
-      <c r="EG16" s="41" t="n"/>
-      <c r="EH16" s="41" t="n"/>
-      <c r="EI16" s="41" t="n"/>
-      <c r="EJ16" s="41" t="n"/>
-      <c r="EK16" s="41" t="n"/>
-      <c r="EL16" s="41" t="n"/>
-      <c r="EM16" s="41" t="n"/>
-      <c r="EN16" s="41" t="n"/>
-      <c r="EO16" s="41" t="n"/>
-      <c r="EP16" s="41" t="n"/>
-      <c r="EQ16" s="41" t="n"/>
-      <c r="ER16" s="41" t="n"/>
-      <c r="ES16" s="41" t="n"/>
-      <c r="ET16" s="41" t="n"/>
-      <c r="EU16" s="41" t="n"/>
-      <c r="EV16" s="41" t="n"/>
-      <c r="EW16" s="41" t="n"/>
-      <c r="EX16" s="41" t="n"/>
-      <c r="EY16" s="41" t="n"/>
-      <c r="EZ16" s="41" t="n"/>
-      <c r="FA16" s="41" t="n"/>
-      <c r="FB16" s="41" t="n"/>
-      <c r="FC16" s="41" t="n"/>
-      <c r="FD16" s="41" t="n"/>
-      <c r="FE16" s="41" t="n"/>
-      <c r="FF16" s="41" t="n"/>
-      <c r="FG16" s="41" t="n"/>
-      <c r="FH16" s="41" t="n"/>
-      <c r="FI16" s="41" t="n"/>
-      <c r="FJ16" s="41" t="n"/>
-    </row>
-    <row r="17" ht="13.8" customHeight="1" s="42">
-      <c r="A17" s="41" t="n"/>
-      <c r="B17" s="41" t="n"/>
-      <c r="C17" s="41" t="n"/>
-      <c r="D17" s="41" t="n"/>
-      <c r="E17" s="41" t="n"/>
-      <c r="F17" s="41" t="n"/>
-      <c r="H17" s="41" t="n"/>
-      <c r="I17" s="41" t="n"/>
-      <c r="J17" s="41" t="n"/>
-      <c r="K17" s="41" t="n"/>
-      <c r="L17" s="41" t="n"/>
-      <c r="M17" s="41" t="n"/>
-      <c r="N17" s="41" t="n"/>
-      <c r="O17" s="41" t="n"/>
-      <c r="P17" s="41" t="n"/>
-      <c r="Q17" s="41" t="n"/>
-      <c r="R17" s="41" t="n"/>
-      <c r="S17" s="41" t="n"/>
-      <c r="T17" s="41" t="n"/>
-      <c r="U17" s="41" t="n"/>
-      <c r="V17" s="41" t="n"/>
-      <c r="W17" s="41" t="n"/>
-      <c r="X17" s="41" t="n"/>
-      <c r="Y17" s="41" t="n"/>
-      <c r="Z17" s="41" t="n"/>
-      <c r="AA17" s="41" t="n"/>
-      <c r="AB17" s="41" t="n"/>
-      <c r="AC17" s="41" t="n"/>
-      <c r="AD17" s="41" t="n"/>
-      <c r="AE17" s="41" t="n"/>
-      <c r="AF17" s="41" t="n"/>
-      <c r="AG17" s="41" t="n"/>
-      <c r="AH17" s="41" t="n"/>
-      <c r="AI17" s="41" t="n"/>
-      <c r="AJ17" s="41" t="n"/>
-      <c r="AK17" s="41" t="n"/>
-      <c r="AL17" s="41" t="n"/>
-      <c r="AM17" s="41" t="n"/>
-      <c r="AN17" s="41" t="n"/>
-      <c r="AO17" s="41" t="n"/>
-      <c r="AP17" s="41" t="n"/>
-      <c r="AQ17" s="41" t="n"/>
-      <c r="AR17" s="41" t="n"/>
-      <c r="AS17" s="41" t="n"/>
-      <c r="AT17" s="41" t="n"/>
-      <c r="AU17" s="41" t="n"/>
-      <c r="AV17" s="41" t="n"/>
-      <c r="AW17" s="41" t="n"/>
-      <c r="AX17" s="41" t="n"/>
-      <c r="AY17" s="41" t="n"/>
-      <c r="AZ17" s="41" t="n"/>
-      <c r="BA17" s="41" t="n"/>
-      <c r="BB17" s="41" t="n"/>
-      <c r="BC17" s="41" t="n"/>
-      <c r="BD17" s="41" t="n"/>
-      <c r="BE17" s="41" t="n"/>
-      <c r="BF17" s="41" t="n"/>
-      <c r="BG17" s="41" t="n"/>
-      <c r="BH17" s="41" t="n"/>
-      <c r="BI17" s="41" t="n"/>
-      <c r="BJ17" s="41" t="n"/>
-      <c r="BK17" s="41" t="n"/>
-      <c r="BL17" s="41" t="n"/>
-      <c r="BM17" s="41" t="n"/>
-      <c r="BN17" s="41" t="n"/>
-      <c r="BO17" s="41" t="n"/>
-      <c r="BP17" s="41" t="n"/>
-      <c r="BQ17" s="41" t="n"/>
-      <c r="BR17" s="41" t="n"/>
-      <c r="BS17" s="41" t="n"/>
-      <c r="BT17" s="41" t="n"/>
-      <c r="BU17" s="41" t="n"/>
-      <c r="BV17" s="41" t="n"/>
-      <c r="BW17" s="41" t="n"/>
-      <c r="BX17" s="41" t="n"/>
-      <c r="BY17" s="41" t="n"/>
-      <c r="BZ17" s="41" t="n"/>
-      <c r="CA17" s="41" t="n"/>
-      <c r="CB17" s="41" t="n"/>
-      <c r="CC17" s="41" t="n"/>
-      <c r="CD17" s="41" t="n"/>
-      <c r="CE17" s="41" t="n"/>
-      <c r="CF17" s="41" t="n"/>
-      <c r="CG17" s="41" t="n"/>
-      <c r="CH17" s="41" t="n"/>
-      <c r="CI17" s="41" t="n"/>
-      <c r="CJ17" s="41" t="n"/>
-      <c r="CK17" s="41" t="n"/>
-      <c r="CL17" s="41" t="n"/>
-      <c r="CM17" s="41" t="n"/>
-      <c r="CN17" s="41" t="n"/>
-      <c r="CO17" s="41" t="n"/>
-      <c r="CP17" s="41" t="n"/>
-      <c r="CQ17" s="41" t="n"/>
-      <c r="CR17" s="41" t="n"/>
-      <c r="CS17" s="41" t="n"/>
-      <c r="CT17" s="41" t="n"/>
-      <c r="CU17" s="41" t="n"/>
-      <c r="CV17" s="41" t="n"/>
-      <c r="CW17" s="41" t="n"/>
-      <c r="CX17" s="41" t="n"/>
-      <c r="CY17" s="41" t="n"/>
-      <c r="CZ17" s="41" t="n"/>
-      <c r="DA17" s="41" t="n"/>
-      <c r="DB17" s="41" t="n"/>
-      <c r="DC17" s="41" t="n"/>
-      <c r="DD17" s="41" t="n"/>
-      <c r="DE17" s="41" t="n"/>
-      <c r="DF17" s="41" t="n"/>
-      <c r="DG17" s="41" t="n"/>
-      <c r="DH17" s="41" t="n"/>
-      <c r="DI17" s="41" t="n"/>
-      <c r="DJ17" s="41" t="n"/>
-      <c r="DK17" s="41" t="n"/>
-      <c r="DL17" s="41" t="n"/>
-      <c r="DM17" s="41" t="n"/>
-      <c r="DN17" s="41" t="n"/>
-      <c r="DO17" s="41" t="n"/>
-      <c r="DP17" s="41" t="n"/>
-      <c r="DQ17" s="41" t="n"/>
-      <c r="DR17" s="41" t="n"/>
-      <c r="DS17" s="41" t="n"/>
-      <c r="DT17" s="41" t="n"/>
-      <c r="DU17" s="41" t="n"/>
-      <c r="DV17" s="41" t="n"/>
-      <c r="DW17" s="41" t="n"/>
-      <c r="DX17" s="41" t="n"/>
-      <c r="DY17" s="41" t="n"/>
-      <c r="DZ17" s="41" t="n"/>
-      <c r="EA17" s="41" t="n"/>
-      <c r="EB17" s="41" t="n"/>
-      <c r="EC17" s="41" t="n"/>
-      <c r="ED17" s="41" t="n"/>
-      <c r="EE17" s="41" t="n"/>
-      <c r="EF17" s="41" t="n"/>
-      <c r="EG17" s="41" t="n"/>
-      <c r="EH17" s="41" t="n"/>
-      <c r="EI17" s="41" t="n"/>
-      <c r="EJ17" s="41" t="n"/>
-      <c r="EK17" s="41" t="n"/>
-      <c r="EL17" s="41" t="n"/>
-      <c r="EM17" s="41" t="n"/>
-      <c r="EN17" s="41" t="n"/>
-      <c r="EO17" s="41" t="n"/>
-      <c r="EP17" s="41" t="n"/>
-      <c r="EQ17" s="41" t="n"/>
-      <c r="ER17" s="41" t="n"/>
-      <c r="ES17" s="41" t="n"/>
-      <c r="ET17" s="41" t="n"/>
-      <c r="EU17" s="41" t="n"/>
-      <c r="EV17" s="41" t="n"/>
-      <c r="EW17" s="41" t="n"/>
-      <c r="EX17" s="41" t="n"/>
-      <c r="EY17" s="41" t="n"/>
-      <c r="EZ17" s="41" t="n"/>
-      <c r="FA17" s="41" t="n"/>
-      <c r="FB17" s="41" t="n"/>
-      <c r="FC17" s="41" t="n"/>
-      <c r="FD17" s="41" t="n"/>
-      <c r="FE17" s="41" t="n"/>
-      <c r="FF17" s="41" t="n"/>
-      <c r="FG17" s="41" t="n"/>
-      <c r="FH17" s="41" t="n"/>
-      <c r="FI17" s="41" t="n"/>
-      <c r="FJ17" s="41" t="n"/>
-    </row>
-    <row r="18" ht="13.8" customHeight="1" s="42">
-      <c r="A18" s="41" t="n"/>
-      <c r="B18" s="41" t="n"/>
-      <c r="C18" s="41" t="n"/>
-      <c r="D18" s="41" t="n"/>
-      <c r="E18" s="41" t="n"/>
-      <c r="F18" s="41" t="n"/>
-      <c r="H18" s="41" t="n"/>
-      <c r="I18" s="41" t="n"/>
-      <c r="J18" s="41" t="n"/>
-      <c r="K18" s="41" t="n"/>
-      <c r="L18" s="41" t="n"/>
-      <c r="M18" s="41" t="n"/>
-      <c r="N18" s="41" t="n"/>
-      <c r="O18" s="41" t="n"/>
-      <c r="P18" s="41" t="n"/>
-      <c r="Q18" s="41" t="n"/>
-      <c r="R18" s="41" t="n"/>
-      <c r="S18" s="41" t="n"/>
-      <c r="T18" s="41" t="n"/>
-      <c r="U18" s="41" t="n"/>
-      <c r="V18" s="41" t="n"/>
-      <c r="W18" s="41" t="n"/>
-      <c r="X18" s="41" t="n"/>
-      <c r="Y18" s="41" t="n"/>
-      <c r="Z18" s="41" t="n"/>
-      <c r="AA18" s="41" t="n"/>
-      <c r="AB18" s="41" t="n"/>
-      <c r="AC18" s="41" t="n"/>
-      <c r="AD18" s="41" t="n"/>
-      <c r="AE18" s="41" t="n"/>
-      <c r="AF18" s="41" t="n"/>
-      <c r="AG18" s="41" t="n"/>
-      <c r="AH18" s="41" t="n"/>
-      <c r="AI18" s="41" t="n"/>
-      <c r="AJ18" s="41" t="n"/>
-      <c r="AK18" s="41" t="n"/>
-      <c r="AL18" s="41" t="n"/>
-      <c r="AM18" s="41" t="n"/>
-      <c r="AN18" s="41" t="n"/>
-      <c r="AO18" s="41" t="n"/>
-      <c r="AP18" s="41" t="n"/>
-      <c r="AQ18" s="41" t="n"/>
-      <c r="AR18" s="41" t="n"/>
-      <c r="AS18" s="41" t="n"/>
-      <c r="AT18" s="41" t="n"/>
-      <c r="AU18" s="41" t="n"/>
-      <c r="AV18" s="41" t="n"/>
-      <c r="AW18" s="41" t="n"/>
-      <c r="AX18" s="41" t="n"/>
-      <c r="AY18" s="41" t="n"/>
-      <c r="AZ18" s="41" t="n"/>
-      <c r="BA18" s="41" t="n"/>
-      <c r="BB18" s="41" t="n"/>
-      <c r="BC18" s="41" t="n"/>
-      <c r="BD18" s="41" t="n"/>
-      <c r="BE18" s="41" t="n"/>
-      <c r="BF18" s="41" t="n"/>
-      <c r="BG18" s="41" t="n"/>
-      <c r="BH18" s="41" t="n"/>
-      <c r="BI18" s="41" t="n"/>
-      <c r="BJ18" s="41" t="n"/>
-      <c r="BK18" s="41" t="n"/>
-      <c r="BL18" s="41" t="n"/>
-      <c r="BM18" s="41" t="n"/>
-      <c r="BN18" s="41" t="n"/>
-      <c r="BO18" s="41" t="n"/>
-      <c r="BP18" s="41" t="n"/>
-      <c r="BQ18" s="41" t="n"/>
-      <c r="BR18" s="41" t="n"/>
-      <c r="BS18" s="41" t="n"/>
-      <c r="BT18" s="41" t="n"/>
-      <c r="BU18" s="41" t="n"/>
-      <c r="BV18" s="41" t="n"/>
-      <c r="BW18" s="41" t="n"/>
-      <c r="BX18" s="41" t="n"/>
-      <c r="BY18" s="41" t="n"/>
-      <c r="BZ18" s="41" t="n"/>
-      <c r="CA18" s="41" t="n"/>
-      <c r="CB18" s="41" t="n"/>
-      <c r="CC18" s="41" t="n"/>
-      <c r="CD18" s="41" t="n"/>
-      <c r="CE18" s="41" t="n"/>
-      <c r="CF18" s="41" t="n"/>
-      <c r="CG18" s="41" t="n"/>
-      <c r="CH18" s="41" t="n"/>
-      <c r="CI18" s="41" t="n"/>
-      <c r="CJ18" s="41" t="n"/>
-      <c r="CK18" s="41" t="n"/>
-      <c r="CL18" s="41" t="n"/>
-      <c r="CM18" s="41" t="n"/>
-      <c r="CN18" s="41" t="n"/>
-      <c r="CO18" s="41" t="n"/>
-      <c r="CP18" s="41" t="n"/>
-      <c r="CQ18" s="41" t="n"/>
-      <c r="CR18" s="41" t="n"/>
-      <c r="CS18" s="41" t="n"/>
-      <c r="CT18" s="41" t="n"/>
-      <c r="CU18" s="41" t="n"/>
-      <c r="CV18" s="41" t="n"/>
-      <c r="CW18" s="41" t="n"/>
-      <c r="CX18" s="41" t="n"/>
-      <c r="CY18" s="41" t="n"/>
-      <c r="CZ18" s="41" t="n"/>
-      <c r="DA18" s="41" t="n"/>
-      <c r="DB18" s="41" t="n"/>
-      <c r="DC18" s="41" t="n"/>
-      <c r="DD18" s="41" t="n"/>
-      <c r="DE18" s="41" t="n"/>
-      <c r="DF18" s="41" t="n"/>
-      <c r="DG18" s="41" t="n"/>
-      <c r="DH18" s="41" t="n"/>
-      <c r="DI18" s="41" t="n"/>
-      <c r="DJ18" s="41" t="n"/>
-      <c r="DK18" s="41" t="n"/>
-      <c r="DL18" s="41" t="n"/>
-      <c r="DM18" s="41" t="n"/>
-      <c r="DN18" s="41" t="n"/>
-      <c r="DO18" s="41" t="n"/>
-      <c r="DP18" s="41" t="n"/>
-      <c r="DQ18" s="41" t="n"/>
-      <c r="DR18" s="41" t="n"/>
-      <c r="DS18" s="41" t="n"/>
-      <c r="DT18" s="41" t="n"/>
-      <c r="DU18" s="41" t="n"/>
-      <c r="DV18" s="41" t="n"/>
-      <c r="DW18" s="41" t="n"/>
-      <c r="DX18" s="41" t="n"/>
-      <c r="DY18" s="41" t="n"/>
-      <c r="DZ18" s="41" t="n"/>
-      <c r="EA18" s="41" t="n"/>
-      <c r="EB18" s="41" t="n"/>
-      <c r="EC18" s="41" t="n"/>
-      <c r="ED18" s="41" t="n"/>
-      <c r="EE18" s="41" t="n"/>
-      <c r="EF18" s="41" t="n"/>
-      <c r="EG18" s="41" t="n"/>
-      <c r="EH18" s="41" t="n"/>
-      <c r="EI18" s="41" t="n"/>
-      <c r="EJ18" s="41" t="n"/>
-      <c r="EK18" s="41" t="n"/>
-      <c r="EL18" s="41" t="n"/>
-      <c r="EM18" s="41" t="n"/>
-      <c r="EN18" s="41" t="n"/>
-      <c r="EO18" s="41" t="n"/>
-      <c r="EP18" s="41" t="n"/>
-      <c r="EQ18" s="41" t="n"/>
-      <c r="ER18" s="41" t="n"/>
-      <c r="ES18" s="41" t="n"/>
-      <c r="ET18" s="41" t="n"/>
-      <c r="EU18" s="41" t="n"/>
-      <c r="EV18" s="41" t="n"/>
-      <c r="EW18" s="41" t="n"/>
-      <c r="EX18" s="41" t="n"/>
-      <c r="EY18" s="41" t="n"/>
-      <c r="EZ18" s="41" t="n"/>
-      <c r="FA18" s="41" t="n"/>
-      <c r="FB18" s="41" t="n"/>
-      <c r="FC18" s="41" t="n"/>
-      <c r="FD18" s="41" t="n"/>
-      <c r="FE18" s="41" t="n"/>
-      <c r="FF18" s="41" t="n"/>
-      <c r="FG18" s="41" t="n"/>
-      <c r="FH18" s="41" t="n"/>
-      <c r="FI18" s="41" t="n"/>
-      <c r="FJ18" s="41" t="n"/>
-    </row>
-    <row r="19" ht="13.8" customHeight="1" s="42">
-      <c r="A19" s="41" t="n"/>
-      <c r="B19" s="41" t="n"/>
-      <c r="C19" s="41" t="n"/>
-      <c r="D19" s="41" t="n"/>
-      <c r="E19" s="41" t="n"/>
-      <c r="F19" s="41" t="n"/>
-      <c r="H19" s="41" t="n"/>
-      <c r="I19" s="41" t="n"/>
-      <c r="J19" s="41" t="n"/>
-      <c r="K19" s="41" t="n"/>
-      <c r="L19" s="41" t="n"/>
-      <c r="M19" s="41" t="n"/>
-      <c r="N19" s="41" t="n"/>
-      <c r="O19" s="41" t="n"/>
-      <c r="P19" s="41" t="n"/>
-      <c r="Q19" s="41" t="n"/>
-      <c r="R19" s="41" t="n"/>
-      <c r="S19" s="41" t="n"/>
-      <c r="T19" s="41" t="n"/>
-      <c r="U19" s="41" t="n"/>
-      <c r="V19" s="41" t="n"/>
-      <c r="W19" s="41" t="n"/>
-      <c r="X19" s="41" t="n"/>
-      <c r="Y19" s="41" t="n"/>
-      <c r="Z19" s="41" t="n"/>
-      <c r="AA19" s="41" t="n"/>
-      <c r="AB19" s="41" t="n"/>
-      <c r="AC19" s="41" t="n"/>
-      <c r="AD19" s="41" t="n"/>
-      <c r="AE19" s="41" t="n"/>
-      <c r="AF19" s="41" t="n"/>
-      <c r="AG19" s="41" t="n"/>
-      <c r="AH19" s="41" t="n"/>
-      <c r="AI19" s="41" t="n"/>
-      <c r="AJ19" s="41" t="n"/>
-      <c r="AK19" s="41" t="n"/>
-      <c r="AL19" s="41" t="n"/>
-      <c r="AM19" s="41" t="n"/>
-      <c r="AN19" s="41" t="n"/>
-      <c r="AO19" s="41" t="n"/>
-      <c r="AP19" s="41" t="n"/>
-      <c r="AQ19" s="41" t="n"/>
-      <c r="AR19" s="41" t="n"/>
-      <c r="AS19" s="41" t="n"/>
-      <c r="AT19" s="41" t="n"/>
-      <c r="AU19" s="41" t="n"/>
-      <c r="AV19" s="41" t="n"/>
-      <c r="AW19" s="41" t="n"/>
-      <c r="AX19" s="41" t="n"/>
-      <c r="AY19" s="41" t="n"/>
-      <c r="AZ19" s="41" t="n"/>
-      <c r="BA19" s="41" t="n"/>
-      <c r="BB19" s="41" t="n"/>
-      <c r="BC19" s="41" t="n"/>
-      <c r="BD19" s="41" t="n"/>
-      <c r="BE19" s="41" t="n"/>
-      <c r="BF19" s="41" t="n"/>
-      <c r="BG19" s="41" t="n"/>
-      <c r="BH19" s="41" t="n"/>
-      <c r="BI19" s="41" t="n"/>
-      <c r="BJ19" s="41" t="n"/>
-      <c r="BK19" s="41" t="n"/>
-      <c r="BL19" s="41" t="n"/>
-      <c r="BM19" s="41" t="n"/>
-      <c r="BN19" s="41" t="n"/>
-      <c r="BO19" s="41" t="n"/>
-      <c r="BP19" s="41" t="n"/>
-      <c r="BQ19" s="41" t="n"/>
-      <c r="BR19" s="41" t="n"/>
-      <c r="BS19" s="41" t="n"/>
-      <c r="BT19" s="41" t="n"/>
-      <c r="BU19" s="41" t="n"/>
-      <c r="BV19" s="41" t="n"/>
-      <c r="BW19" s="41" t="n"/>
-      <c r="BX19" s="41" t="n"/>
-      <c r="BY19" s="41" t="n"/>
-      <c r="BZ19" s="41" t="n"/>
-      <c r="CA19" s="41" t="n"/>
-      <c r="CB19" s="41" t="n"/>
-      <c r="CC19" s="41" t="n"/>
-      <c r="CD19" s="41" t="n"/>
-      <c r="CE19" s="41" t="n"/>
-      <c r="CF19" s="41" t="n"/>
-      <c r="CG19" s="41" t="n"/>
-      <c r="CH19" s="41" t="n"/>
-      <c r="CI19" s="41" t="n"/>
-      <c r="CJ19" s="41" t="n"/>
-      <c r="CK19" s="41" t="n"/>
-      <c r="CL19" s="41" t="n"/>
-      <c r="CM19" s="41" t="n"/>
-      <c r="CN19" s="41" t="n"/>
-      <c r="CO19" s="41" t="n"/>
-      <c r="CP19" s="41" t="n"/>
-      <c r="CQ19" s="41" t="n"/>
-      <c r="CR19" s="41" t="n"/>
-      <c r="CS19" s="41" t="n"/>
-      <c r="CT19" s="41" t="n"/>
-      <c r="CU19" s="41" t="n"/>
-      <c r="CV19" s="41" t="n"/>
-      <c r="CW19" s="41" t="n"/>
-      <c r="CX19" s="41" t="n"/>
-      <c r="CY19" s="41" t="n"/>
-      <c r="CZ19" s="41" t="n"/>
-      <c r="DA19" s="41" t="n"/>
-      <c r="DB19" s="41" t="n"/>
-      <c r="DC19" s="41" t="n"/>
-      <c r="DD19" s="41" t="n"/>
-      <c r="DE19" s="41" t="n"/>
-      <c r="DF19" s="41" t="n"/>
-      <c r="DG19" s="41" t="n"/>
-      <c r="DH19" s="41" t="n"/>
-      <c r="DI19" s="41" t="n"/>
-      <c r="DJ19" s="41" t="n"/>
-      <c r="DK19" s="41" t="n"/>
-      <c r="DL19" s="41" t="n"/>
-      <c r="DM19" s="41" t="n"/>
-      <c r="DN19" s="41" t="n"/>
-      <c r="DO19" s="41" t="n"/>
-      <c r="DP19" s="41" t="n"/>
-      <c r="DQ19" s="41" t="n"/>
-      <c r="DR19" s="41" t="n"/>
-      <c r="DS19" s="41" t="n"/>
-      <c r="DT19" s="41" t="n"/>
-      <c r="DU19" s="41" t="n"/>
-      <c r="DV19" s="41" t="n"/>
-      <c r="DW19" s="41" t="n"/>
-      <c r="DX19" s="41" t="n"/>
-      <c r="DY19" s="41" t="n"/>
-      <c r="DZ19" s="41" t="n"/>
-      <c r="EA19" s="41" t="n"/>
-      <c r="EB19" s="41" t="n"/>
-      <c r="EC19" s="41" t="n"/>
-      <c r="ED19" s="41" t="n"/>
-      <c r="EE19" s="41" t="n"/>
-      <c r="EF19" s="41" t="n"/>
-      <c r="EG19" s="41" t="n"/>
-      <c r="EH19" s="41" t="n"/>
-      <c r="EI19" s="41" t="n"/>
-      <c r="EJ19" s="41" t="n"/>
-      <c r="EK19" s="41" t="n"/>
-      <c r="EL19" s="41" t="n"/>
-      <c r="EM19" s="41" t="n"/>
-      <c r="EN19" s="41" t="n"/>
-      <c r="EO19" s="41" t="n"/>
-      <c r="EP19" s="41" t="n"/>
-      <c r="EQ19" s="41" t="n"/>
-      <c r="ER19" s="41" t="n"/>
-      <c r="ES19" s="41" t="n"/>
-      <c r="ET19" s="41" t="n"/>
-      <c r="EU19" s="41" t="n"/>
-      <c r="EV19" s="41" t="n"/>
-      <c r="EW19" s="41" t="n"/>
-      <c r="EX19" s="41" t="n"/>
-      <c r="EY19" s="41" t="n"/>
-      <c r="EZ19" s="41" t="n"/>
-      <c r="FA19" s="41" t="n"/>
-      <c r="FB19" s="41" t="n"/>
-      <c r="FC19" s="41" t="n"/>
-      <c r="FD19" s="41" t="n"/>
-      <c r="FE19" s="41" t="n"/>
-      <c r="FF19" s="41" t="n"/>
-      <c r="FG19" s="41" t="n"/>
-      <c r="FH19" s="41" t="n"/>
-      <c r="FI19" s="41" t="n"/>
-      <c r="FJ19" s="41" t="n"/>
-    </row>
-    <row r="20" ht="13.8" customHeight="1" s="42">
-      <c r="A20" s="41" t="n"/>
-      <c r="B20" s="41" t="n"/>
-      <c r="C20" s="41" t="n"/>
-      <c r="D20" s="41" t="n"/>
-      <c r="E20" s="41" t="n"/>
-      <c r="F20" s="41" t="n"/>
-      <c r="H20" s="41" t="n"/>
-      <c r="I20" s="41" t="n"/>
-      <c r="J20" s="41" t="n"/>
-      <c r="K20" s="41" t="n"/>
-      <c r="L20" s="41" t="n"/>
-      <c r="M20" s="41" t="n"/>
-      <c r="N20" s="41" t="n"/>
-      <c r="O20" s="41" t="n"/>
-      <c r="P20" s="41" t="n"/>
-      <c r="Q20" s="41" t="n"/>
-      <c r="R20" s="41" t="n"/>
-      <c r="S20" s="41" t="n"/>
-      <c r="T20" s="41" t="n"/>
-      <c r="U20" s="41" t="n"/>
-      <c r="V20" s="41" t="n"/>
-      <c r="W20" s="41" t="n"/>
-      <c r="X20" s="41" t="n"/>
-      <c r="Y20" s="41" t="n"/>
-      <c r="Z20" s="41" t="n"/>
-      <c r="AA20" s="41" t="n"/>
-      <c r="AB20" s="41" t="n"/>
-      <c r="AC20" s="41" t="n"/>
-      <c r="AD20" s="41" t="n"/>
-      <c r="AE20" s="41" t="n"/>
-      <c r="AF20" s="41" t="n"/>
-      <c r="AG20" s="41" t="n"/>
-      <c r="AH20" s="41" t="n"/>
-      <c r="AI20" s="41" t="n"/>
-      <c r="AJ20" s="41" t="n"/>
-      <c r="AK20" s="41" t="n"/>
-      <c r="AL20" s="41" t="n"/>
-      <c r="AM20" s="41" t="n"/>
-      <c r="AN20" s="41" t="n"/>
-      <c r="AO20" s="41" t="n"/>
-      <c r="AP20" s="41" t="n"/>
-      <c r="AQ20" s="41" t="n"/>
-      <c r="AR20" s="41" t="n"/>
-      <c r="AS20" s="41" t="n"/>
-      <c r="AT20" s="41" t="n"/>
-      <c r="AU20" s="41" t="n"/>
-      <c r="AV20" s="41" t="n"/>
-      <c r="AW20" s="41" t="n"/>
-      <c r="AX20" s="41" t="n"/>
-      <c r="AY20" s="41" t="n"/>
-      <c r="AZ20" s="41" t="n"/>
-      <c r="BA20" s="41" t="n"/>
-      <c r="BB20" s="41" t="n"/>
-      <c r="BC20" s="41" t="n"/>
-      <c r="BD20" s="41" t="n"/>
-      <c r="BE20" s="41" t="n"/>
-      <c r="BF20" s="41" t="n"/>
-      <c r="BG20" s="41" t="n"/>
-      <c r="BH20" s="41" t="n"/>
-      <c r="BI20" s="41" t="n"/>
-      <c r="BJ20" s="41" t="n"/>
-      <c r="BK20" s="41" t="n"/>
-      <c r="BL20" s="41" t="n"/>
-      <c r="BM20" s="41" t="n"/>
-      <c r="BN20" s="41" t="n"/>
-      <c r="BO20" s="41" t="n"/>
-      <c r="BP20" s="41" t="n"/>
-      <c r="BQ20" s="41" t="n"/>
-      <c r="BR20" s="41" t="n"/>
-      <c r="BS20" s="41" t="n"/>
-      <c r="BT20" s="41" t="n"/>
-      <c r="BU20" s="41" t="n"/>
-      <c r="BV20" s="41" t="n"/>
-      <c r="BW20" s="41" t="n"/>
-      <c r="BX20" s="41" t="n"/>
-      <c r="BY20" s="41" t="n"/>
-      <c r="BZ20" s="41" t="n"/>
-      <c r="CA20" s="41" t="n"/>
-      <c r="CB20" s="41" t="n"/>
-      <c r="CC20" s="41" t="n"/>
-      <c r="CD20" s="41" t="n"/>
-      <c r="CE20" s="41" t="n"/>
-      <c r="CF20" s="41" t="n"/>
-      <c r="CG20" s="41" t="n"/>
-      <c r="CH20" s="41" t="n"/>
-      <c r="CI20" s="41" t="n"/>
-      <c r="CJ20" s="41" t="n"/>
-      <c r="CK20" s="41" t="n"/>
-      <c r="CL20" s="41" t="n"/>
-      <c r="CM20" s="41" t="n"/>
-      <c r="CN20" s="41" t="n"/>
-      <c r="CO20" s="41" t="n"/>
-      <c r="CP20" s="41" t="n"/>
-      <c r="CQ20" s="41" t="n"/>
-      <c r="CR20" s="41" t="n"/>
-      <c r="CS20" s="41" t="n"/>
-      <c r="CT20" s="41" t="n"/>
-      <c r="CU20" s="41" t="n"/>
-      <c r="CV20" s="41" t="n"/>
-      <c r="CW20" s="41" t="n"/>
-      <c r="CX20" s="41" t="n"/>
-      <c r="CY20" s="41" t="n"/>
-      <c r="CZ20" s="41" t="n"/>
-      <c r="DA20" s="41" t="n"/>
-      <c r="DB20" s="41" t="n"/>
-      <c r="DC20" s="41" t="n"/>
-      <c r="DD20" s="41" t="n"/>
-      <c r="DE20" s="41" t="n"/>
-      <c r="DF20" s="41" t="n"/>
-      <c r="DG20" s="41" t="n"/>
-      <c r="DH20" s="41" t="n"/>
-      <c r="DI20" s="41" t="n"/>
-      <c r="DJ20" s="41" t="n"/>
-      <c r="DK20" s="41" t="n"/>
-      <c r="DL20" s="41" t="n"/>
-      <c r="DM20" s="41" t="n"/>
-      <c r="DN20" s="41" t="n"/>
-      <c r="DO20" s="41" t="n"/>
-      <c r="DP20" s="41" t="n"/>
-      <c r="DQ20" s="41" t="n"/>
-      <c r="DR20" s="41" t="n"/>
-      <c r="DS20" s="41" t="n"/>
-      <c r="DT20" s="41" t="n"/>
-      <c r="DU20" s="41" t="n"/>
-      <c r="DV20" s="41" t="n"/>
-      <c r="DW20" s="41" t="n"/>
-      <c r="DX20" s="41" t="n"/>
-      <c r="DY20" s="41" t="n"/>
-      <c r="DZ20" s="41" t="n"/>
-      <c r="EA20" s="41" t="n"/>
-      <c r="EB20" s="41" t="n"/>
-      <c r="EC20" s="41" t="n"/>
-      <c r="ED20" s="41" t="n"/>
-      <c r="EE20" s="41" t="n"/>
-      <c r="EF20" s="41" t="n"/>
-      <c r="EG20" s="41" t="n"/>
-      <c r="EH20" s="41" t="n"/>
-      <c r="EI20" s="41" t="n"/>
-      <c r="EJ20" s="41" t="n"/>
-      <c r="EK20" s="41" t="n"/>
-      <c r="EL20" s="41" t="n"/>
-      <c r="EM20" s="41" t="n"/>
-      <c r="EN20" s="41" t="n"/>
-      <c r="EO20" s="41" t="n"/>
-      <c r="EP20" s="41" t="n"/>
-      <c r="EQ20" s="41" t="n"/>
-      <c r="ER20" s="41" t="n"/>
-      <c r="ES20" s="41" t="n"/>
-      <c r="ET20" s="41" t="n"/>
-      <c r="EU20" s="41" t="n"/>
-      <c r="EV20" s="41" t="n"/>
-      <c r="EW20" s="41" t="n"/>
-      <c r="EX20" s="41" t="n"/>
-      <c r="EY20" s="41" t="n"/>
-      <c r="EZ20" s="41" t="n"/>
-      <c r="FA20" s="41" t="n"/>
-      <c r="FB20" s="41" t="n"/>
-      <c r="FC20" s="41" t="n"/>
-      <c r="FD20" s="41" t="n"/>
-      <c r="FE20" s="41" t="n"/>
-      <c r="FF20" s="41" t="n"/>
-      <c r="FG20" s="41" t="n"/>
-      <c r="FH20" s="41" t="n"/>
-      <c r="FI20" s="41" t="n"/>
-      <c r="FJ20" s="41" t="n"/>
-    </row>
-    <row r="21" ht="13.8" customHeight="1" s="42">
-      <c r="A21" s="41" t="n"/>
-      <c r="B21" s="41" t="n"/>
-      <c r="C21" s="41" t="n"/>
-      <c r="D21" s="41" t="n"/>
-      <c r="E21" s="41" t="n"/>
-      <c r="F21" s="41" t="n"/>
-      <c r="H21" s="41" t="n"/>
-      <c r="I21" s="41" t="n"/>
-      <c r="J21" s="41" t="n"/>
-      <c r="K21" s="41" t="n"/>
-      <c r="L21" s="41" t="n"/>
-      <c r="M21" s="41" t="n"/>
-      <c r="N21" s="41" t="n"/>
-      <c r="O21" s="41" t="n"/>
-      <c r="P21" s="41" t="n"/>
-      <c r="Q21" s="41" t="n"/>
-      <c r="R21" s="41" t="n"/>
-      <c r="S21" s="41" t="n"/>
-      <c r="T21" s="41" t="n"/>
-      <c r="U21" s="41" t="n"/>
-      <c r="V21" s="41" t="n"/>
-      <c r="W21" s="41" t="n"/>
-      <c r="X21" s="41" t="n"/>
-      <c r="Y21" s="41" t="n"/>
-      <c r="Z21" s="41" t="n"/>
-      <c r="AA21" s="41" t="n"/>
-      <c r="AB21" s="41" t="n"/>
-      <c r="AC21" s="41" t="n"/>
-      <c r="AD21" s="41" t="n"/>
-      <c r="AE21" s="41" t="n"/>
-      <c r="AF21" s="41" t="n"/>
-      <c r="AG21" s="41" t="n"/>
-      <c r="AH21" s="41" t="n"/>
-      <c r="AI21" s="41" t="n"/>
-      <c r="AJ21" s="41" t="n"/>
-      <c r="AK21" s="41" t="n"/>
-      <c r="AL21" s="41" t="n"/>
-      <c r="AM21" s="41" t="n"/>
-      <c r="AN21" s="41" t="n"/>
-      <c r="AO21" s="41" t="n"/>
-      <c r="AP21" s="41" t="n"/>
-      <c r="AQ21" s="41" t="n"/>
-      <c r="AR21" s="41" t="n"/>
-      <c r="AS21" s="41" t="n"/>
-      <c r="AT21" s="41" t="n"/>
-      <c r="AU21" s="41" t="n"/>
-      <c r="AV21" s="41" t="n"/>
-      <c r="AW21" s="41" t="n"/>
-      <c r="AX21" s="41" t="n"/>
-      <c r="AY21" s="41" t="n"/>
-      <c r="AZ21" s="41" t="n"/>
-      <c r="BA21" s="41" t="n"/>
-      <c r="BB21" s="41" t="n"/>
-      <c r="BC21" s="41" t="n"/>
-      <c r="BD21" s="41" t="n"/>
-      <c r="BE21" s="41" t="n"/>
-      <c r="BF21" s="41" t="n"/>
-      <c r="BG21" s="41" t="n"/>
-      <c r="BH21" s="41" t="n"/>
-      <c r="BI21" s="41" t="n"/>
-      <c r="BJ21" s="41" t="n"/>
-      <c r="BK21" s="41" t="n"/>
-      <c r="BL21" s="41" t="n"/>
-      <c r="BM21" s="41" t="n"/>
-      <c r="BN21" s="41" t="n"/>
-      <c r="BO21" s="41" t="n"/>
-      <c r="BP21" s="41" t="n"/>
-      <c r="BQ21" s="41" t="n"/>
-      <c r="BR21" s="41" t="n"/>
-      <c r="BS21" s="41" t="n"/>
-      <c r="BT21" s="41" t="n"/>
-      <c r="BU21" s="41" t="n"/>
-      <c r="BV21" s="41" t="n"/>
-      <c r="BW21" s="41" t="n"/>
-      <c r="BX21" s="41" t="n"/>
-      <c r="BY21" s="41" t="n"/>
-      <c r="BZ21" s="41" t="n"/>
-      <c r="CA21" s="41" t="n"/>
-      <c r="CB21" s="41" t="n"/>
-      <c r="CC21" s="41" t="n"/>
-      <c r="CD21" s="41" t="n"/>
-      <c r="CE21" s="41" t="n"/>
-      <c r="CF21" s="41" t="n"/>
-      <c r="CG21" s="41" t="n"/>
-      <c r="CH21" s="41" t="n"/>
-      <c r="CI21" s="41" t="n"/>
-      <c r="CJ21" s="41" t="n"/>
-      <c r="CK21" s="41" t="n"/>
-      <c r="CL21" s="41" t="n"/>
-      <c r="CM21" s="41" t="n"/>
-      <c r="CN21" s="41" t="n"/>
-      <c r="CO21" s="41" t="n"/>
-      <c r="CP21" s="41" t="n"/>
-      <c r="CQ21" s="41" t="n"/>
-      <c r="CR21" s="41" t="n"/>
-      <c r="CS21" s="41" t="n"/>
-      <c r="CT21" s="41" t="n"/>
-      <c r="CU21" s="41" t="n"/>
-      <c r="CV21" s="41" t="n"/>
-      <c r="CW21" s="41" t="n"/>
-      <c r="CX21" s="41" t="n"/>
-      <c r="CY21" s="41" t="n"/>
-      <c r="CZ21" s="41" t="n"/>
-      <c r="DA21" s="41" t="n"/>
-      <c r="DB21" s="41" t="n"/>
-      <c r="DC21" s="41" t="n"/>
-      <c r="DD21" s="41" t="n"/>
-      <c r="DE21" s="41" t="n"/>
-      <c r="DF21" s="41" t="n"/>
-      <c r="DG21" s="41" t="n"/>
-      <c r="DH21" s="41" t="n"/>
-      <c r="DI21" s="41" t="n"/>
-      <c r="DJ21" s="41" t="n"/>
-      <c r="DK21" s="41" t="n"/>
-      <c r="DL21" s="41" t="n"/>
-      <c r="DM21" s="41" t="n"/>
-      <c r="DN21" s="41" t="n"/>
-      <c r="DO21" s="41" t="n"/>
-      <c r="DP21" s="41" t="n"/>
-      <c r="DQ21" s="41" t="n"/>
-      <c r="DR21" s="41" t="n"/>
-      <c r="DS21" s="41" t="n"/>
-      <c r="DT21" s="41" t="n"/>
-      <c r="DU21" s="41" t="n"/>
-      <c r="DV21" s="41" t="n"/>
-      <c r="DW21" s="41" t="n"/>
-      <c r="DX21" s="41" t="n"/>
-      <c r="DY21" s="41" t="n"/>
-      <c r="DZ21" s="41" t="n"/>
-      <c r="EA21" s="41" t="n"/>
-      <c r="EB21" s="41" t="n"/>
-      <c r="EC21" s="41" t="n"/>
-      <c r="ED21" s="41" t="n"/>
-      <c r="EE21" s="41" t="n"/>
-      <c r="EF21" s="41" t="n"/>
-      <c r="EG21" s="41" t="n"/>
-      <c r="EH21" s="41" t="n"/>
-      <c r="EI21" s="41" t="n"/>
-      <c r="EJ21" s="41" t="n"/>
-      <c r="EK21" s="41" t="n"/>
-      <c r="EL21" s="41" t="n"/>
-      <c r="EM21" s="41" t="n"/>
-      <c r="EN21" s="41" t="n"/>
-      <c r="EO21" s="41" t="n"/>
-      <c r="EP21" s="41" t="n"/>
-      <c r="EQ21" s="41" t="n"/>
-      <c r="ER21" s="41" t="n"/>
-      <c r="ES21" s="41" t="n"/>
-      <c r="ET21" s="41" t="n"/>
-      <c r="EU21" s="41" t="n"/>
-      <c r="EV21" s="41" t="n"/>
-      <c r="EW21" s="41" t="n"/>
-      <c r="EX21" s="41" t="n"/>
-      <c r="EY21" s="41" t="n"/>
-      <c r="EZ21" s="41" t="n"/>
-      <c r="FA21" s="41" t="n"/>
-      <c r="FB21" s="41" t="n"/>
-      <c r="FC21" s="41" t="n"/>
-      <c r="FD21" s="41" t="n"/>
-      <c r="FE21" s="41" t="n"/>
-      <c r="FF21" s="41" t="n"/>
-      <c r="FG21" s="41" t="n"/>
-      <c r="FH21" s="41" t="n"/>
-      <c r="FI21" s="41" t="n"/>
-      <c r="FJ21" s="41" t="n"/>
-    </row>
-    <row r="22" ht="13.8" customHeight="1" s="42">
-      <c r="A22" s="41" t="n"/>
-      <c r="B22" s="41" t="n"/>
-      <c r="C22" s="41" t="n"/>
-      <c r="D22" s="41" t="n"/>
-      <c r="E22" s="41" t="n"/>
-      <c r="F22" s="41" t="n"/>
-      <c r="H22" s="41" t="n"/>
-      <c r="I22" s="41" t="n"/>
-      <c r="J22" s="41" t="n"/>
-      <c r="K22" s="41" t="n"/>
-      <c r="L22" s="41" t="n"/>
-      <c r="M22" s="41" t="n"/>
-      <c r="N22" s="41" t="n"/>
-      <c r="O22" s="41" t="n"/>
-      <c r="P22" s="41" t="n"/>
-      <c r="Q22" s="41" t="n"/>
-      <c r="R22" s="41" t="n"/>
-      <c r="S22" s="41" t="n"/>
-      <c r="T22" s="41" t="n"/>
-      <c r="U22" s="41" t="n"/>
-      <c r="V22" s="41" t="n"/>
-      <c r="W22" s="41" t="n"/>
-      <c r="X22" s="41" t="n"/>
-      <c r="Y22" s="41" t="n"/>
-      <c r="Z22" s="41" t="n"/>
-      <c r="AA22" s="41" t="n"/>
-      <c r="AB22" s="41" t="n"/>
-      <c r="AC22" s="41" t="n"/>
-      <c r="AD22" s="41" t="n"/>
-      <c r="AE22" s="41" t="n"/>
-      <c r="AF22" s="41" t="n"/>
-      <c r="AG22" s="41" t="n"/>
-      <c r="AH22" s="41" t="n"/>
-      <c r="AI22" s="41" t="n"/>
-      <c r="AJ22" s="41" t="n"/>
-      <c r="AK22" s="41" t="n"/>
-      <c r="AL22" s="41" t="n"/>
-      <c r="AM22" s="41" t="n"/>
-      <c r="AN22" s="41" t="n"/>
-      <c r="AO22" s="41" t="n"/>
-      <c r="AP22" s="41" t="n"/>
-      <c r="AQ22" s="41" t="n"/>
-      <c r="AR22" s="41" t="n"/>
-      <c r="AS22" s="41" t="n"/>
-      <c r="AT22" s="41" t="n"/>
-      <c r="AU22" s="41" t="n"/>
-      <c r="AV22" s="41" t="n"/>
-      <c r="AW22" s="41" t="n"/>
-      <c r="AX22" s="41" t="n"/>
-      <c r="AY22" s="41" t="n"/>
-      <c r="AZ22" s="41" t="n"/>
-      <c r="BA22" s="41" t="n"/>
-      <c r="BB22" s="41" t="n"/>
-      <c r="BC22" s="41" t="n"/>
-      <c r="BD22" s="41" t="n"/>
-      <c r="BE22" s="41" t="n"/>
-      <c r="BF22" s="41" t="n"/>
-      <c r="BG22" s="41" t="n"/>
-      <c r="BH22" s="41" t="n"/>
-      <c r="BI22" s="41" t="n"/>
-      <c r="BJ22" s="41" t="n"/>
-      <c r="BK22" s="41" t="n"/>
-      <c r="BL22" s="41" t="n"/>
-      <c r="BM22" s="41" t="n"/>
-      <c r="BN22" s="41" t="n"/>
-      <c r="BO22" s="41" t="n"/>
-      <c r="BP22" s="41" t="n"/>
-      <c r="BQ22" s="41" t="n"/>
-      <c r="BR22" s="41" t="n"/>
-      <c r="BS22" s="41" t="n"/>
-      <c r="BT22" s="41" t="n"/>
-      <c r="BU22" s="41" t="n"/>
-      <c r="BV22" s="41" t="n"/>
-      <c r="BW22" s="41" t="n"/>
-      <c r="BX22" s="41" t="n"/>
-      <c r="BY22" s="41" t="n"/>
-      <c r="BZ22" s="41" t="n"/>
-      <c r="CA22" s="41" t="n"/>
-      <c r="CB22" s="41" t="n"/>
-      <c r="CC22" s="41" t="n"/>
-      <c r="CD22" s="41" t="n"/>
-      <c r="CE22" s="41" t="n"/>
-      <c r="CF22" s="41" t="n"/>
-      <c r="CG22" s="41" t="n"/>
-      <c r="CH22" s="41" t="n"/>
-      <c r="CI22" s="41" t="n"/>
-      <c r="CJ22" s="41" t="n"/>
-      <c r="CK22" s="41" t="n"/>
-      <c r="CL22" s="41" t="n"/>
-      <c r="CM22" s="41" t="n"/>
-      <c r="CN22" s="41" t="n"/>
-      <c r="CO22" s="41" t="n"/>
-      <c r="CP22" s="41" t="n"/>
-      <c r="CQ22" s="41" t="n"/>
-      <c r="CR22" s="41" t="n"/>
-      <c r="CS22" s="41" t="n"/>
-      <c r="CT22" s="41" t="n"/>
-      <c r="CU22" s="41" t="n"/>
-      <c r="CV22" s="41" t="n"/>
-      <c r="CW22" s="41" t="n"/>
-      <c r="CX22" s="41" t="n"/>
-      <c r="CY22" s="41" t="n"/>
-      <c r="CZ22" s="41" t="n"/>
-      <c r="DA22" s="41" t="n"/>
-      <c r="DB22" s="41" t="n"/>
-      <c r="DC22" s="41" t="n"/>
-      <c r="DD22" s="41" t="n"/>
-      <c r="DE22" s="41" t="n"/>
-      <c r="DF22" s="41" t="n"/>
-      <c r="DG22" s="41" t="n"/>
-      <c r="DH22" s="41" t="n"/>
-      <c r="DI22" s="41" t="n"/>
-      <c r="DJ22" s="41" t="n"/>
-      <c r="DK22" s="41" t="n"/>
-      <c r="DL22" s="41" t="n"/>
-      <c r="DM22" s="41" t="n"/>
-      <c r="DN22" s="41" t="n"/>
-      <c r="DO22" s="41" t="n"/>
-      <c r="DP22" s="41" t="n"/>
-      <c r="DQ22" s="41" t="n"/>
-      <c r="DR22" s="41" t="n"/>
-      <c r="DS22" s="41" t="n"/>
-      <c r="DT22" s="41" t="n"/>
-      <c r="DU22" s="41" t="n"/>
-      <c r="DV22" s="41" t="n"/>
-      <c r="DW22" s="41" t="n"/>
-      <c r="DX22" s="41" t="n"/>
-      <c r="DY22" s="41" t="n"/>
-      <c r="DZ22" s="41" t="n"/>
-      <c r="EA22" s="41" t="n"/>
-      <c r="EB22" s="41" t="n"/>
-      <c r="EC22" s="41" t="n"/>
-      <c r="ED22" s="41" t="n"/>
-      <c r="EE22" s="41" t="n"/>
-      <c r="EF22" s="41" t="n"/>
-      <c r="EG22" s="41" t="n"/>
-      <c r="EH22" s="41" t="n"/>
-      <c r="EI22" s="41" t="n"/>
-      <c r="EJ22" s="41" t="n"/>
-      <c r="EK22" s="41" t="n"/>
-      <c r="EL22" s="41" t="n"/>
-      <c r="EM22" s="41" t="n"/>
-      <c r="EN22" s="41" t="n"/>
-      <c r="EO22" s="41" t="n"/>
-      <c r="EP22" s="41" t="n"/>
-      <c r="EQ22" s="41" t="n"/>
-      <c r="ER22" s="41" t="n"/>
-      <c r="ES22" s="41" t="n"/>
-      <c r="ET22" s="41" t="n"/>
-      <c r="EU22" s="41" t="n"/>
-      <c r="EV22" s="41" t="n"/>
-      <c r="EW22" s="41" t="n"/>
-      <c r="EX22" s="41" t="n"/>
-      <c r="EY22" s="41" t="n"/>
-      <c r="EZ22" s="41" t="n"/>
-      <c r="FA22" s="41" t="n"/>
-      <c r="FB22" s="41" t="n"/>
-      <c r="FC22" s="41" t="n"/>
-      <c r="FD22" s="41" t="n"/>
-      <c r="FE22" s="41" t="n"/>
-      <c r="FF22" s="41" t="n"/>
-      <c r="FG22" s="41" t="n"/>
-      <c r="FH22" s="41" t="n"/>
-      <c r="FI22" s="41" t="n"/>
-      <c r="FJ22" s="41" t="n"/>
-    </row>
-    <row r="23" ht="13.8" customHeight="1" s="42">
-      <c r="A23" s="41" t="n"/>
-      <c r="B23" s="41" t="n"/>
-      <c r="C23" s="41" t="n"/>
-      <c r="D23" s="41" t="n"/>
-      <c r="E23" s="41" t="n"/>
-      <c r="F23" s="41" t="n"/>
-      <c r="H23" s="41" t="n"/>
-      <c r="I23" s="41" t="n"/>
-      <c r="J23" s="41" t="n"/>
-      <c r="K23" s="41" t="n"/>
-      <c r="L23" s="41" t="n"/>
-      <c r="M23" s="41" t="n"/>
-      <c r="N23" s="41" t="n"/>
-      <c r="O23" s="41" t="n"/>
-      <c r="P23" s="41" t="n"/>
-      <c r="Q23" s="41" t="n"/>
-      <c r="R23" s="41" t="n"/>
-      <c r="S23" s="41" t="n"/>
-      <c r="T23" s="41" t="n"/>
-      <c r="U23" s="41" t="n"/>
-      <c r="V23" s="41" t="n"/>
-      <c r="W23" s="41" t="n"/>
-      <c r="X23" s="41" t="n"/>
-      <c r="Y23" s="41" t="n"/>
-      <c r="Z23" s="41" t="n"/>
-      <c r="AA23" s="41" t="n"/>
-      <c r="AB23" s="41" t="n"/>
-      <c r="AC23" s="41" t="n"/>
-      <c r="AD23" s="41" t="n"/>
-      <c r="AE23" s="41" t="n"/>
-      <c r="AF23" s="41" t="n"/>
-      <c r="AG23" s="41" t="n"/>
-      <c r="AH23" s="41" t="n"/>
-      <c r="AI23" s="41" t="n"/>
-      <c r="AJ23" s="41" t="n"/>
-      <c r="AK23" s="41" t="n"/>
-      <c r="AL23" s="41" t="n"/>
-      <c r="AM23" s="41" t="n"/>
-      <c r="AN23" s="41" t="n"/>
-      <c r="AO23" s="41" t="n"/>
-      <c r="AP23" s="41" t="n"/>
-      <c r="AQ23" s="41" t="n"/>
-      <c r="AR23" s="41" t="n"/>
-      <c r="AS23" s="41" t="n"/>
-      <c r="AT23" s="41" t="n"/>
-      <c r="AU23" s="41" t="n"/>
-      <c r="AV23" s="41" t="n"/>
-      <c r="AW23" s="41" t="n"/>
-      <c r="AX23" s="41" t="n"/>
-      <c r="AY23" s="41" t="n"/>
-      <c r="AZ23" s="41" t="n"/>
-      <c r="BA23" s="41" t="n"/>
-      <c r="BB23" s="41" t="n"/>
-      <c r="BC23" s="41" t="n"/>
-      <c r="BD23" s="41" t="n"/>
-      <c r="BE23" s="41" t="n"/>
-      <c r="BF23" s="41" t="n"/>
-      <c r="BG23" s="41" t="n"/>
-      <c r="BH23" s="41" t="n"/>
-      <c r="BI23" s="41" t="n"/>
-      <c r="BJ23" s="41" t="n"/>
-      <c r="BK23" s="41" t="n"/>
-      <c r="BL23" s="41" t="n"/>
-      <c r="BM23" s="41" t="n"/>
-      <c r="BN23" s="41" t="n"/>
-      <c r="BO23" s="41" t="n"/>
-      <c r="BP23" s="41" t="n"/>
-      <c r="BQ23" s="41" t="n"/>
-      <c r="BR23" s="41" t="n"/>
-      <c r="BS23" s="41" t="n"/>
-      <c r="BT23" s="41" t="n"/>
-      <c r="BU23" s="41" t="n"/>
-      <c r="BV23" s="41" t="n"/>
-      <c r="BW23" s="41" t="n"/>
-      <c r="BX23" s="41" t="n"/>
-      <c r="BY23" s="41" t="n"/>
-      <c r="BZ23" s="41" t="n"/>
-      <c r="CA23" s="41" t="n"/>
-      <c r="CB23" s="41" t="n"/>
-      <c r="CC23" s="41" t="n"/>
-      <c r="CD23" s="41" t="n"/>
-      <c r="CE23" s="41" t="n"/>
-      <c r="CF23" s="41" t="n"/>
-      <c r="CG23" s="41" t="n"/>
-      <c r="CH23" s="41" t="n"/>
-      <c r="CI23" s="41" t="n"/>
-      <c r="CJ23" s="41" t="n"/>
-      <c r="CK23" s="41" t="n"/>
-      <c r="CL23" s="41" t="n"/>
-      <c r="CM23" s="41" t="n"/>
-      <c r="CN23" s="41" t="n"/>
-      <c r="CO23" s="41" t="n"/>
-      <c r="CP23" s="41" t="n"/>
-      <c r="CQ23" s="41" t="n"/>
-      <c r="CR23" s="41" t="n"/>
-      <c r="CS23" s="41" t="n"/>
-      <c r="CT23" s="41" t="n"/>
-      <c r="CU23" s="41" t="n"/>
-      <c r="CV23" s="41" t="n"/>
-      <c r="CW23" s="41" t="n"/>
-      <c r="CX23" s="41" t="n"/>
-      <c r="CY23" s="41" t="n"/>
-      <c r="CZ23" s="41" t="n"/>
-      <c r="DA23" s="41" t="n"/>
-      <c r="DB23" s="41" t="n"/>
-      <c r="DC23" s="41" t="n"/>
-      <c r="DD23" s="41" t="n"/>
-      <c r="DE23" s="41" t="n"/>
-      <c r="DF23" s="41" t="n"/>
-      <c r="DG23" s="41" t="n"/>
-      <c r="DH23" s="41" t="n"/>
-      <c r="DI23" s="41" t="n"/>
-      <c r="DJ23" s="41" t="n"/>
-      <c r="DK23" s="41" t="n"/>
-      <c r="DL23" s="41" t="n"/>
-      <c r="DM23" s="41" t="n"/>
-      <c r="DN23" s="41" t="n"/>
-      <c r="DO23" s="41" t="n"/>
-      <c r="DP23" s="41" t="n"/>
-      <c r="DQ23" s="41" t="n"/>
-      <c r="DR23" s="41" t="n"/>
-      <c r="DS23" s="41" t="n"/>
-      <c r="DT23" s="41" t="n"/>
-      <c r="DU23" s="41" t="n"/>
-      <c r="DV23" s="41" t="n"/>
-      <c r="DW23" s="41" t="n"/>
-      <c r="DX23" s="41" t="n"/>
-      <c r="DY23" s="41" t="n"/>
-      <c r="DZ23" s="41" t="n"/>
-      <c r="EA23" s="41" t="n"/>
-      <c r="EB23" s="41" t="n"/>
-      <c r="EC23" s="41" t="n"/>
-      <c r="ED23" s="41" t="n"/>
-      <c r="EE23" s="41" t="n"/>
-      <c r="EF23" s="41" t="n"/>
-      <c r="EG23" s="41" t="n"/>
-      <c r="EH23" s="41" t="n"/>
-      <c r="EI23" s="41" t="n"/>
-      <c r="EJ23" s="41" t="n"/>
-      <c r="EK23" s="41" t="n"/>
-      <c r="EL23" s="41" t="n"/>
-      <c r="EM23" s="41" t="n"/>
-      <c r="EN23" s="41" t="n"/>
-      <c r="EO23" s="41" t="n"/>
-      <c r="EP23" s="41" t="n"/>
-      <c r="EQ23" s="41" t="n"/>
-      <c r="ER23" s="41" t="n"/>
-      <c r="ES23" s="41" t="n"/>
-      <c r="ET23" s="41" t="n"/>
-      <c r="EU23" s="41" t="n"/>
-      <c r="EV23" s="41" t="n"/>
-      <c r="EW23" s="41" t="n"/>
-      <c r="EX23" s="41" t="n"/>
-      <c r="EY23" s="41" t="n"/>
-      <c r="EZ23" s="41" t="n"/>
-      <c r="FA23" s="41" t="n"/>
-      <c r="FB23" s="41" t="n"/>
-      <c r="FC23" s="41" t="n"/>
-      <c r="FD23" s="41" t="n"/>
-      <c r="FE23" s="41" t="n"/>
-      <c r="FF23" s="41" t="n"/>
-      <c r="FG23" s="41" t="n"/>
-      <c r="FH23" s="41" t="n"/>
-      <c r="FI23" s="41" t="n"/>
-      <c r="FJ23" s="41" t="n"/>
-    </row>
-    <row r="24" ht="13.8" customHeight="1" s="42">
-      <c r="A24" s="41" t="n"/>
-      <c r="B24" s="41" t="n"/>
-      <c r="C24" s="41" t="n"/>
-      <c r="D24" s="41" t="n"/>
-      <c r="E24" s="41" t="n"/>
-      <c r="F24" s="41" t="n"/>
-      <c r="H24" s="41" t="n"/>
-      <c r="I24" s="41" t="n"/>
-      <c r="J24" s="41" t="n"/>
-      <c r="K24" s="41" t="n"/>
-      <c r="L24" s="41" t="n"/>
-      <c r="M24" s="41" t="n"/>
-      <c r="N24" s="41" t="n"/>
-      <c r="O24" s="41" t="n"/>
-      <c r="P24" s="41" t="n"/>
-      <c r="Q24" s="41" t="n"/>
-      <c r="R24" s="41" t="n"/>
-      <c r="S24" s="41" t="n"/>
-      <c r="T24" s="41" t="n"/>
-      <c r="U24" s="41" t="n"/>
-      <c r="V24" s="41" t="n"/>
-      <c r="W24" s="41" t="n"/>
-      <c r="X24" s="41" t="n"/>
-      <c r="Y24" s="41" t="n"/>
-      <c r="Z24" s="41" t="n"/>
-      <c r="AA24" s="41" t="n"/>
-      <c r="AB24" s="41" t="n"/>
-      <c r="AC24" s="41" t="n"/>
-      <c r="AD24" s="41" t="n"/>
-      <c r="AE24" s="41" t="n"/>
-      <c r="AF24" s="41" t="n"/>
-      <c r="AG24" s="41" t="n"/>
-      <c r="AH24" s="41" t="n"/>
-      <c r="AI24" s="41" t="n"/>
-      <c r="AJ24" s="41" t="n"/>
-      <c r="AK24" s="41" t="n"/>
-      <c r="AL24" s="41" t="n"/>
-      <c r="AM24" s="41" t="n"/>
-      <c r="AN24" s="41" t="n"/>
-      <c r="AO24" s="41" t="n"/>
-      <c r="AP24" s="41" t="n"/>
-      <c r="AQ24" s="41" t="n"/>
-      <c r="AR24" s="41" t="n"/>
-      <c r="AS24" s="41" t="n"/>
-      <c r="AT24" s="41" t="n"/>
-      <c r="AU24" s="41" t="n"/>
-      <c r="AV24" s="41" t="n"/>
-      <c r="AW24" s="41" t="n"/>
-      <c r="AX24" s="41" t="n"/>
-      <c r="AY24" s="41" t="n"/>
-      <c r="AZ24" s="41" t="n"/>
-      <c r="BA24" s="41" t="n"/>
-      <c r="BB24" s="41" t="n"/>
-      <c r="BC24" s="41" t="n"/>
-      <c r="BD24" s="41" t="n"/>
-      <c r="BE24" s="41" t="n"/>
-      <c r="BF24" s="41" t="n"/>
-      <c r="BG24" s="41" t="n"/>
-      <c r="BH24" s="41" t="n"/>
-      <c r="BI24" s="41" t="n"/>
-      <c r="BJ24" s="41" t="n"/>
-      <c r="BK24" s="41" t="n"/>
-      <c r="BL24" s="41" t="n"/>
-      <c r="BM24" s="41" t="n"/>
-      <c r="BN24" s="41" t="n"/>
-      <c r="BO24" s="41" t="n"/>
-      <c r="BP24" s="41" t="n"/>
-      <c r="BQ24" s="41" t="n"/>
-      <c r="BR24" s="41" t="n"/>
-      <c r="BS24" s="41" t="n"/>
-      <c r="BT24" s="41" t="n"/>
-      <c r="BU24" s="41" t="n"/>
-      <c r="BV24" s="41" t="n"/>
-      <c r="BW24" s="41" t="n"/>
-      <c r="BX24" s="41" t="n"/>
-      <c r="BY24" s="41" t="n"/>
-      <c r="BZ24" s="41" t="n"/>
-      <c r="CA24" s="41" t="n"/>
-      <c r="CB24" s="41" t="n"/>
-      <c r="CC24" s="41" t="n"/>
-      <c r="CD24" s="41" t="n"/>
-      <c r="CE24" s="41" t="n"/>
-      <c r="CF24" s="41" t="n"/>
-      <c r="CG24" s="41" t="n"/>
-      <c r="CH24" s="41" t="n"/>
-      <c r="CI24" s="41" t="n"/>
-      <c r="CJ24" s="41" t="n"/>
-      <c r="CK24" s="41" t="n"/>
-      <c r="CL24" s="41" t="n"/>
-      <c r="CM24" s="41" t="n"/>
-      <c r="CN24" s="41" t="n"/>
-      <c r="CO24" s="41" t="n"/>
-      <c r="CP24" s="41" t="n"/>
-      <c r="CQ24" s="41" t="n"/>
-      <c r="CR24" s="41" t="n"/>
-      <c r="CS24" s="41" t="n"/>
-      <c r="CT24" s="41" t="n"/>
-      <c r="CU24" s="41" t="n"/>
-      <c r="CV24" s="41" t="n"/>
-      <c r="CW24" s="41" t="n"/>
-      <c r="CX24" s="41" t="n"/>
-      <c r="CY24" s="41" t="n"/>
-      <c r="CZ24" s="41" t="n"/>
-      <c r="DA24" s="41" t="n"/>
-      <c r="DB24" s="41" t="n"/>
-      <c r="DC24" s="41" t="n"/>
-      <c r="DD24" s="41" t="n"/>
-      <c r="DE24" s="41" t="n"/>
-      <c r="DF24" s="41" t="n"/>
-      <c r="DG24" s="41" t="n"/>
-      <c r="DH24" s="41" t="n"/>
-      <c r="DI24" s="41" t="n"/>
-      <c r="DJ24" s="41" t="n"/>
-      <c r="DK24" s="41" t="n"/>
-      <c r="DL24" s="41" t="n"/>
-      <c r="DM24" s="41" t="n"/>
-      <c r="DN24" s="41" t="n"/>
-      <c r="DO24" s="41" t="n"/>
-      <c r="DP24" s="41" t="n"/>
-      <c r="DQ24" s="41" t="n"/>
-      <c r="DR24" s="41" t="n"/>
-      <c r="DS24" s="41" t="n"/>
-      <c r="DT24" s="41" t="n"/>
-      <c r="DU24" s="41" t="n"/>
-      <c r="DV24" s="41" t="n"/>
-      <c r="DW24" s="41" t="n"/>
-      <c r="DX24" s="41" t="n"/>
-      <c r="DY24" s="41" t="n"/>
-      <c r="DZ24" s="41" t="n"/>
-      <c r="EA24" s="41" t="n"/>
-      <c r="EB24" s="41" t="n"/>
-      <c r="EC24" s="41" t="n"/>
-      <c r="ED24" s="41" t="n"/>
-      <c r="EE24" s="41" t="n"/>
-      <c r="EF24" s="41" t="n"/>
-      <c r="EG24" s="41" t="n"/>
-      <c r="EH24" s="41" t="n"/>
-      <c r="EI24" s="41" t="n"/>
-      <c r="EJ24" s="41" t="n"/>
-      <c r="EK24" s="41" t="n"/>
-      <c r="EL24" s="41" t="n"/>
-      <c r="EM24" s="41" t="n"/>
-      <c r="EN24" s="41" t="n"/>
-      <c r="EO24" s="41" t="n"/>
-      <c r="EP24" s="41" t="n"/>
-      <c r="EQ24" s="41" t="n"/>
-      <c r="ER24" s="41" t="n"/>
-      <c r="ES24" s="41" t="n"/>
-      <c r="ET24" s="41" t="n"/>
-      <c r="EU24" s="41" t="n"/>
-      <c r="EV24" s="41" t="n"/>
-      <c r="EW24" s="41" t="n"/>
-      <c r="EX24" s="41" t="n"/>
-      <c r="EY24" s="41" t="n"/>
-      <c r="EZ24" s="41" t="n"/>
-      <c r="FA24" s="41" t="n"/>
-      <c r="FB24" s="41" t="n"/>
-      <c r="FC24" s="41" t="n"/>
-      <c r="FD24" s="41" t="n"/>
-      <c r="FE24" s="41" t="n"/>
-      <c r="FF24" s="41" t="n"/>
-      <c r="FG24" s="41" t="n"/>
-      <c r="FH24" s="41" t="n"/>
-      <c r="FI24" s="41" t="n"/>
-      <c r="FJ24" s="41" t="n"/>
-    </row>
+    <row r="8" ht="13.8" customHeight="1" s="42"/>
+    <row r="9" ht="13.8" customHeight="1" s="42"/>
+    <row r="10" ht="13.8" customHeight="1" s="42"/>
+    <row r="11" ht="13.8" customHeight="1" s="42"/>
+    <row r="12" ht="13.8" customHeight="1" s="42"/>
+    <row r="13" ht="13.8" customHeight="1" s="42"/>
+    <row r="14" ht="13.8" customHeight="1" s="42"/>
+    <row r="15" ht="13.8" customHeight="1" s="42"/>
+    <row r="16" ht="13.8" customHeight="1" s="42"/>
+    <row r="17" ht="13.8" customHeight="1" s="42"/>
+    <row r="18" ht="13.8" customHeight="1" s="42"/>
+    <row r="19" ht="13.8" customHeight="1" s="42"/>
+    <row r="20" ht="13.8" customHeight="1" s="42"/>
+    <row r="21" ht="13.8" customHeight="1" s="42"/>
+    <row r="22" ht="13.8" customHeight="1" s="42"/>
+    <row r="23" ht="13.8" customHeight="1" s="42"/>
+    <row r="24" ht="13.8" customHeight="1" s="42"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9219,7 +6207,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:FJ6 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
arreglo de las fechas de nutricion
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -65,7 +65,7 @@
       <sz val="9"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -144,12 +144,6 @@
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF3838"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -226,7 +220,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -410,7 +404,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -591,9 +585,6 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -959,11 +950,11 @@
   </sheetPr>
   <dimension ref="A1:FX12"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="FG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="FJ20" activeCellId="0" sqref="FJ20"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="EO1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="ER7" activeCellId="0" sqref="ER7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="12.96" customWidth="1" style="62" min="1" max="166"/>
   </cols>
@@ -6770,9 +6761,9 @@
           <t>1</t>
         </is>
       </c>
-      <c r="EQ8" s="124" t="inlineStr">
-        <is>
-          <t xml:space="preserve">y hora de </t>
+      <c r="EQ8" s="62" t="inlineStr">
+        <is>
+          <t>2021-04-15</t>
         </is>
       </c>
       <c r="ER8" s="62" t="inlineStr">
@@ -6802,7 +6793,7 @@
       </c>
       <c r="EW8" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">y hora de </t>
+          <t>2021 -1801</t>
         </is>
       </c>
       <c r="EX8" s="62" t="inlineStr">
@@ -7598,7 +7589,7 @@
       </c>
       <c r="EW9" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">y hora de </t>
+          <t>2021-01-04</t>
         </is>
       </c>
       <c r="EX9" s="62" t="inlineStr">
@@ -8359,42 +8350,42 @@
       </c>
       <c r="EP10" s="62" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EQ10" s="62" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="ER10" s="62" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES10" s="62" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ET10" s="62" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EU10" s="62" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV10" s="62" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="EQ10" s="62" t="inlineStr">
-        <is>
-          <t>2021-02-08</t>
-        </is>
-      </c>
-      <c r="ER10" s="62" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="ES10" s="62" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="ET10" s="62" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="EU10" s="62" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="EV10" s="62" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="EW10" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">y hora de </t>
+          <t>2021-02-04</t>
         </is>
       </c>
       <c r="EX10" s="62" t="inlineStr">
@@ -9163,12 +9154,12 @@
       </c>
       <c r="EP11" s="62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="EQ11" s="62" t="inlineStr">
         <is>
-          <t>1845-01-01</t>
+          <t>2021-03-23</t>
         </is>
       </c>
       <c r="ER11" s="62" t="inlineStr">
@@ -9994,7 +9985,7 @@
       </c>
       <c r="EW12" s="62" t="inlineStr">
         <is>
-          <t xml:space="preserve">y hora de </t>
+          <t>2021-01-04</t>
         </is>
       </c>
       <c r="EX12" s="62" t="inlineStr">
@@ -10095,7 +10086,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
creacion del ambiente virtual y verificacion de la compatibilidad de las librerias
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -6660,7 +6660,7 @@
       </c>
       <c r="G9" s="143" t="inlineStr">
         <is>
-          <t>1989 -02-10</t>
+          <t>1969 -02-10</t>
         </is>
       </c>
       <c r="H9" s="143" t="inlineStr">
@@ -9167,7 +9167,7 @@
       </c>
       <c r="Q12" s="143" t="inlineStr">
         <is>
-          <t>cb59</t>
+          <t>c859</t>
         </is>
       </c>
       <c r="R12" s="143" t="inlineStr">
@@ -11502,7 +11502,7 @@
       </c>
       <c r="FB14" s="143" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="FC14" s="143" t="inlineStr">
@@ -11517,7 +11517,7 @@
       </c>
       <c r="FE14" s="143" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="FF14" s="143" t="inlineStr">
@@ -14904,7 +14904,7 @@
       </c>
       <c r="Q19" s="143" t="inlineStr">
         <is>
-          <t>c859</t>
+          <t xml:space="preserve">c59 </t>
         </is>
       </c>
       <c r="R19" s="143" t="inlineStr">
@@ -15772,7 +15772,7 @@
       </c>
       <c r="AB20" s="143" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC20" s="143" t="inlineStr">
@@ -16130,17 +16130,17 @@
       </c>
       <c r="CV20" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="CW20" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>98</t>
         </is>
       </c>
       <c r="CX20" s="143" t="inlineStr">
         <is>
-          <t>2021-01-19</t>
+          <t>1845-01-01</t>
         </is>
       </c>
       <c r="CY20" s="143" t="inlineStr">
@@ -16150,12 +16150,12 @@
       </c>
       <c r="CZ20" s="143" t="inlineStr">
         <is>
-          <t>345302</t>
+          <t>98</t>
         </is>
       </c>
       <c r="DA20" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>98</t>
         </is>
       </c>
       <c r="DB20" s="143" t="inlineStr">
@@ -16391,7 +16391,7 @@
       </c>
       <c r="EW20" s="143" t="inlineStr">
         <is>
-          <t>2021-02-11</t>
+          <t>202-02- 11</t>
         </is>
       </c>
       <c r="EX20" s="143" t="inlineStr">
@@ -18227,7 +18227,7 @@
       </c>
       <c r="AB23" s="143" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AC23" s="143" t="inlineStr">
@@ -20565,22 +20565,22 @@
     <row r="26" ht="13.8" customHeight="1" s="73">
       <c r="A26" s="143" t="inlineStr">
         <is>
-          <t>pedro</t>
+          <t>alfredo</t>
         </is>
       </c>
       <c r="B26" s="143" t="inlineStr">
         <is>
-          <t>celestino</t>
+          <t>de</t>
         </is>
       </c>
       <c r="C26" s="143" t="inlineStr">
         <is>
-          <t>guerra</t>
+          <t>jesus</t>
         </is>
       </c>
       <c r="D26" s="143" t="inlineStr">
         <is>
-          <t>guerra</t>
+          <t>brito</t>
         </is>
       </c>
       <c r="E26" s="143" t="inlineStr">
@@ -20590,12 +20590,12 @@
       </c>
       <c r="F26" s="143" t="inlineStr">
         <is>
-          <t>5143043</t>
+          <t>1753652</t>
         </is>
       </c>
       <c r="G26" s="143" t="inlineStr">
         <is>
-          <t>1943 -04-04</t>
+          <t>1937 -10-15</t>
         </is>
       </c>
       <c r="H26" s="143" t="inlineStr">
@@ -20631,7 +20631,7 @@
       </c>
       <c r="O26" s="143" t="inlineStr">
         <is>
-          <t xml:space="preserve">3016842967 </t>
+          <t xml:space="preserve">3004932870 </t>
         </is>
       </c>
       <c r="P26" s="143" t="inlineStr">
@@ -20698,7 +20698,7 @@
       </c>
       <c r="AD26" s="143" t="inlineStr">
         <is>
-          <t>2021-02-01</t>
+          <t>2021-04-26</t>
         </is>
       </c>
       <c r="AE26" s="143" t="inlineStr">
@@ -20733,7 +20733,7 @@
       </c>
       <c r="AK26" s="143" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>11</t>
         </is>
       </c>
       <c r="AL26" s="143" t="inlineStr">
@@ -21386,22 +21386,22 @@
     <row r="27" ht="13.8" customHeight="1" s="73">
       <c r="A27" s="143" t="inlineStr">
         <is>
-          <t>nayibis</t>
+          <t>pedro</t>
         </is>
       </c>
       <c r="B27" s="143" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>celestino</t>
         </is>
       </c>
       <c r="C27" s="143" t="inlineStr">
         <is>
-          <t>morelo</t>
+          <t>guerra</t>
         </is>
       </c>
       <c r="D27" s="143" t="inlineStr">
         <is>
-          <t>marimon</t>
+          <t>guerra</t>
         </is>
       </c>
       <c r="E27" s="143" t="inlineStr">
@@ -21411,22 +21411,22 @@
       </c>
       <c r="F27" s="143" t="inlineStr">
         <is>
-          <t>40925684</t>
+          <t>5143043</t>
         </is>
       </c>
       <c r="G27" s="143" t="inlineStr">
         <is>
-          <t>1971 -01-14</t>
+          <t>1943 -04-04</t>
         </is>
       </c>
       <c r="H27" s="143" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>M</t>
         </is>
       </c>
       <c r="I27" s="143" t="inlineStr">
         <is>
-          <t>9622</t>
+          <t>9629</t>
         </is>
       </c>
       <c r="J27" s="143" t="inlineStr">
@@ -21442,7 +21442,7 @@
       </c>
       <c r="M27" s="143" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>31</t>
         </is>
       </c>
       <c r="N27" s="143" t="inlineStr">
@@ -21452,7 +21452,7 @@
       </c>
       <c r="O27" s="143" t="inlineStr">
         <is>
-          <t xml:space="preserve">3226754735 </t>
+          <t xml:space="preserve">3016842967 </t>
         </is>
       </c>
       <c r="P27" s="143" t="inlineStr">
@@ -21462,12 +21462,12 @@
       </c>
       <c r="Q27" s="143" t="inlineStr">
         <is>
-          <t>c509</t>
+          <t>c61x</t>
         </is>
       </c>
       <c r="R27" s="143" t="inlineStr">
         <is>
-          <t>2017-11-20</t>
+          <t>1800-01-01</t>
         </is>
       </c>
       <c r="S27" s="143" t="inlineStr">
@@ -21494,12 +21494,12 @@
       <c r="X27" s="143" t="n"/>
       <c r="Y27" s="143" t="inlineStr">
         <is>
-          <t>80010054401</t>
+          <t>99</t>
         </is>
       </c>
       <c r="Z27" s="143" t="inlineStr">
         <is>
-          <t>2021-01-19</t>
+          <t>1800-01-01</t>
         </is>
       </c>
       <c r="AA27" s="143" t="inlineStr">
@@ -21509,375 +21509,377 @@
       </c>
       <c r="AB27" s="143" t="inlineStr">
         <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="AC27" s="143" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AD27" s="143" t="inlineStr">
+        <is>
+          <t>2021-02-01</t>
+        </is>
+      </c>
+      <c r="AE27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AF27" s="143" t="inlineStr">
+        <is>
+          <t>1846-01-01</t>
+        </is>
+      </c>
+      <c r="AG27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AH27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AJ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AN27" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO27" s="143" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AP27" s="143" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AC27" s="143" t="inlineStr">
+      <c r="AQ27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AR27" s="143" t="inlineStr">
         <is>
           <t>99</t>
         </is>
       </c>
-      <c r="AD27" s="143" t="inlineStr">
-        <is>
-          <t>2021-04-19</t>
-        </is>
-      </c>
-      <c r="AE27" s="143" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF27" s="143" t="inlineStr">
-        <is>
-          <t>pendiente</t>
-        </is>
-      </c>
-      <c r="AG27" s="143" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AI27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="AJ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AK27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AL27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AM27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="AN27" s="143" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO27" s="143" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AP27" s="143" t="inlineStr">
+      <c r="AS27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AV27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AW27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AX27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AY27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AZ27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BA27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BB27" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BC27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BF27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BX27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CB27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS27" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CT27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU27" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV27" s="143" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AQ27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="AR27" s="143" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="AS27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AT27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="AU27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="AV27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="AW27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="AX27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="AY27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="AZ27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="BA27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="BB27" s="143" t="inlineStr">
-        <is>
-          <t>97</t>
-        </is>
-      </c>
-      <c r="BC27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BD27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BE27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="BF27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BG27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BH27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BI27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BJ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BK27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BL27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BM27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BN27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BO27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BP27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BQ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BR27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BS27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BT27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BU27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BV27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BW27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="BX27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BY27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="BZ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CA27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="CB27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CC27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CD27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CE27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CF27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CG27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CH27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CI27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CJ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CK27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CL27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CM27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CN27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CO27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CP27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CQ27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CR27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CS27" s="143" t="inlineStr">
-        <is>
-          <t>1845-01-01</t>
-        </is>
-      </c>
-      <c r="CT27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CU27" s="143" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="CV27" s="143" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="CW27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>98</t>
         </is>
       </c>
       <c r="CX27" s="143" t="inlineStr">
         <is>
-          <t>2021-01-26</t>
+          <t>1845-01-01</t>
         </is>
       </c>
       <c r="CY27" s="143" t="inlineStr">
@@ -21887,12 +21889,12 @@
       </c>
       <c r="CZ27" s="143" t="inlineStr">
         <is>
-          <t>134530</t>
+          <t>98</t>
         </is>
       </c>
       <c r="DA27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>98</t>
         </is>
       </c>
       <c r="DB27" s="143" t="inlineStr">
@@ -22067,12 +22069,12 @@
       </c>
       <c r="EJ27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EK27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EL27" s="143" t="inlineStr">
@@ -22097,12 +22099,12 @@
       </c>
       <c r="EP27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EQ27" s="143" t="inlineStr">
         <is>
-          <t>2021-03-23</t>
+          <t>1845-01-01</t>
         </is>
       </c>
       <c r="ER27" s="143" t="inlineStr">
@@ -22127,12 +22129,12 @@
       </c>
       <c r="EV27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EW27" s="143" t="inlineStr">
         <is>
-          <t>2021-01-25</t>
+          <t>1845-01-01</t>
         </is>
       </c>
       <c r="EX27" s="143" t="inlineStr">
@@ -22142,7 +22144,7 @@
       </c>
       <c r="EY27" s="143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="EZ27" s="143" t="inlineStr">
@@ -22203,172 +22205,822 @@
       <c r="FK27" s="143" t="n"/>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="73">
-      <c r="A28" s="143" t="n"/>
-      <c r="B28" s="143" t="n"/>
-      <c r="C28" s="143" t="n"/>
-      <c r="D28" s="143" t="n"/>
-      <c r="E28" s="143" t="n"/>
-      <c r="F28" s="143" t="n"/>
-      <c r="G28" s="143" t="n"/>
-      <c r="H28" s="143" t="n"/>
-      <c r="I28" s="143" t="n"/>
-      <c r="J28" s="143" t="n"/>
+      <c r="A28" s="143" t="inlineStr">
+        <is>
+          <t>nayibis</t>
+        </is>
+      </c>
+      <c r="B28" s="143" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="C28" s="143" t="inlineStr">
+        <is>
+          <t>morelo</t>
+        </is>
+      </c>
+      <c r="D28" s="143" t="inlineStr">
+        <is>
+          <t>marimon</t>
+        </is>
+      </c>
+      <c r="E28" s="143" t="inlineStr">
+        <is>
+          <t>cc</t>
+        </is>
+      </c>
+      <c r="F28" s="143" t="inlineStr">
+        <is>
+          <t>40925684</t>
+        </is>
+      </c>
+      <c r="G28" s="143" t="inlineStr">
+        <is>
+          <t>1971 -01-14</t>
+        </is>
+      </c>
+      <c r="H28" s="143" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="I28" s="143" t="inlineStr">
+        <is>
+          <t>9622</t>
+        </is>
+      </c>
+      <c r="J28" s="143" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
       <c r="K28" s="143" t="n"/>
-      <c r="L28" s="143" t="n"/>
-      <c r="M28" s="143" t="n"/>
-      <c r="N28" s="143" t="n"/>
-      <c r="O28" s="143" t="n"/>
-      <c r="P28" s="143" t="n"/>
-      <c r="Q28" s="143" t="n"/>
-      <c r="R28" s="143" t="n"/>
-      <c r="S28" s="143" t="n"/>
-      <c r="T28" s="143" t="n"/>
-      <c r="U28" s="143" t="n"/>
-      <c r="V28" s="143" t="n"/>
+      <c r="L28" s="143" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="M28" s="143" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="N28" s="143" t="inlineStr">
+        <is>
+          <t>44001</t>
+        </is>
+      </c>
+      <c r="O28" s="143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3226754735 </t>
+        </is>
+      </c>
+      <c r="P28" s="143" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="Q28" s="143" t="inlineStr">
+        <is>
+          <t>c509</t>
+        </is>
+      </c>
+      <c r="R28" s="143" t="inlineStr">
+        <is>
+          <t>2017-11-20</t>
+        </is>
+      </c>
+      <c r="S28" s="143" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="T28" s="143" t="inlineStr">
+        <is>
+          <t>1800-01-01</t>
+        </is>
+      </c>
+      <c r="U28" s="143" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="V28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
       <c r="W28" s="143" t="n"/>
       <c r="X28" s="143" t="n"/>
-      <c r="Y28" s="143" t="n"/>
-      <c r="Z28" s="143" t="n"/>
-      <c r="AA28" s="143" t="n"/>
-      <c r="AB28" s="143" t="n"/>
-      <c r="AC28" s="143" t="n"/>
-      <c r="AD28" s="143" t="n"/>
-      <c r="AE28" s="143" t="n"/>
-      <c r="AF28" s="143" t="n"/>
-      <c r="AG28" s="143" t="n"/>
-      <c r="AH28" s="143" t="n"/>
-      <c r="AI28" s="143" t="n"/>
-      <c r="AJ28" s="143" t="n"/>
-      <c r="AK28" s="143" t="n"/>
-      <c r="AL28" s="143" t="n"/>
-      <c r="AM28" s="143" t="n"/>
-      <c r="AN28" s="143" t="n"/>
-      <c r="AO28" s="143" t="n"/>
-      <c r="AP28" s="143" t="n"/>
-      <c r="AQ28" s="143" t="n"/>
-      <c r="AR28" s="143" t="n"/>
-      <c r="AS28" s="143" t="n"/>
-      <c r="AT28" s="143" t="n"/>
-      <c r="AU28" s="143" t="n"/>
-      <c r="AV28" s="143" t="n"/>
-      <c r="AW28" s="143" t="n"/>
-      <c r="AX28" s="143" t="n"/>
-      <c r="AY28" s="143" t="n"/>
-      <c r="AZ28" s="143" t="n"/>
-      <c r="BA28" s="143" t="n"/>
-      <c r="BB28" s="143" t="n"/>
-      <c r="BC28" s="143" t="n"/>
-      <c r="BD28" s="143" t="n"/>
-      <c r="BE28" s="143" t="n"/>
-      <c r="BF28" s="143" t="n"/>
-      <c r="BG28" s="143" t="n"/>
-      <c r="BH28" s="143" t="n"/>
-      <c r="BI28" s="143" t="n"/>
-      <c r="BJ28" s="143" t="n"/>
-      <c r="BK28" s="143" t="n"/>
-      <c r="BL28" s="143" t="n"/>
-      <c r="BM28" s="143" t="n"/>
-      <c r="BN28" s="143" t="n"/>
-      <c r="BO28" s="143" t="n"/>
-      <c r="BP28" s="143" t="n"/>
-      <c r="BQ28" s="143" t="n"/>
-      <c r="BR28" s="143" t="n"/>
-      <c r="BS28" s="143" t="n"/>
-      <c r="BT28" s="143" t="n"/>
-      <c r="BU28" s="143" t="n"/>
-      <c r="BV28" s="143" t="n"/>
-      <c r="BW28" s="143" t="n"/>
-      <c r="BX28" s="143" t="n"/>
-      <c r="BY28" s="143" t="n"/>
-      <c r="BZ28" s="143" t="n"/>
-      <c r="CA28" s="143" t="n"/>
-      <c r="CB28" s="143" t="n"/>
-      <c r="CC28" s="143" t="n"/>
-      <c r="CD28" s="143" t="n"/>
-      <c r="CE28" s="143" t="n"/>
-      <c r="CF28" s="143" t="n"/>
-      <c r="CG28" s="143" t="n"/>
-      <c r="CH28" s="143" t="n"/>
-      <c r="CI28" s="143" t="n"/>
-      <c r="CJ28" s="143" t="n"/>
-      <c r="CK28" s="143" t="n"/>
-      <c r="CL28" s="143" t="n"/>
-      <c r="CM28" s="143" t="n"/>
-      <c r="CN28" s="143" t="n"/>
-      <c r="CO28" s="143" t="n"/>
-      <c r="CP28" s="143" t="n"/>
-      <c r="CQ28" s="143" t="n"/>
-      <c r="CR28" s="143" t="n"/>
-      <c r="CS28" s="143" t="n"/>
-      <c r="CT28" s="143" t="n"/>
-      <c r="CU28" s="143" t="n"/>
-      <c r="CV28" s="143" t="n"/>
-      <c r="CW28" s="143" t="n"/>
-      <c r="CX28" s="143" t="n"/>
-      <c r="CY28" s="143" t="n"/>
-      <c r="CZ28" s="143" t="n"/>
-      <c r="DA28" s="143" t="n"/>
-      <c r="DB28" s="143" t="n"/>
-      <c r="DC28" s="143" t="n"/>
-      <c r="DD28" s="143" t="n"/>
-      <c r="DE28" s="143" t="n"/>
-      <c r="DF28" s="143" t="n"/>
-      <c r="DG28" s="143" t="n"/>
-      <c r="DH28" s="143" t="n"/>
-      <c r="DI28" s="143" t="n"/>
-      <c r="DJ28" s="143" t="n"/>
-      <c r="DK28" s="143" t="n"/>
-      <c r="DL28" s="143" t="n"/>
-      <c r="DM28" s="143" t="n"/>
-      <c r="DN28" s="143" t="n"/>
-      <c r="DO28" s="143" t="n"/>
-      <c r="DP28" s="143" t="n"/>
-      <c r="DQ28" s="143" t="n"/>
-      <c r="DR28" s="143" t="n"/>
-      <c r="DS28" s="143" t="n"/>
-      <c r="DT28" s="143" t="n"/>
-      <c r="DU28" s="143" t="n"/>
-      <c r="DV28" s="143" t="n"/>
-      <c r="DW28" s="143" t="n"/>
-      <c r="DX28" s="143" t="n"/>
-      <c r="DY28" s="143" t="n"/>
-      <c r="DZ28" s="143" t="n"/>
-      <c r="EA28" s="143" t="n"/>
-      <c r="EB28" s="143" t="n"/>
-      <c r="EC28" s="143" t="n"/>
-      <c r="ED28" s="143" t="n"/>
-      <c r="EE28" s="143" t="n"/>
-      <c r="EF28" s="143" t="n"/>
-      <c r="EG28" s="143" t="n"/>
-      <c r="EH28" s="143" t="n"/>
-      <c r="EI28" s="143" t="n"/>
-      <c r="EJ28" s="143" t="n"/>
-      <c r="EK28" s="143" t="n"/>
-      <c r="EL28" s="143" t="n"/>
-      <c r="EM28" s="143" t="n"/>
-      <c r="EN28" s="143" t="n"/>
-      <c r="EO28" s="143" t="n"/>
-      <c r="EP28" s="143" t="n"/>
-      <c r="EQ28" s="143" t="n"/>
-      <c r="ER28" s="143" t="n"/>
-      <c r="ES28" s="143" t="n"/>
-      <c r="ET28" s="143" t="n"/>
-      <c r="EU28" s="143" t="n"/>
-      <c r="EV28" s="143" t="n"/>
-      <c r="EW28" s="143" t="n"/>
-      <c r="EX28" s="143" t="n"/>
-      <c r="EY28" s="143" t="n"/>
-      <c r="EZ28" s="143" t="n"/>
-      <c r="FA28" s="143" t="n"/>
-      <c r="FB28" s="143" t="n"/>
-      <c r="FC28" s="143" t="n"/>
-      <c r="FD28" s="143" t="n"/>
-      <c r="FE28" s="143" t="n"/>
-      <c r="FF28" s="143" t="n"/>
-      <c r="FG28" s="143" t="n"/>
-      <c r="FH28" s="143" t="n"/>
-      <c r="FI28" s="143" t="n"/>
-      <c r="FJ28" s="143" t="n"/>
+      <c r="Y28" s="143" t="inlineStr">
+        <is>
+          <t>80010054401</t>
+        </is>
+      </c>
+      <c r="Z28" s="143" t="inlineStr">
+        <is>
+          <t>2021-01-19</t>
+        </is>
+      </c>
+      <c r="AA28" s="143" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AB28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AC28" s="143" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AD28" s="143" t="inlineStr">
+        <is>
+          <t>2021-04-19</t>
+        </is>
+      </c>
+      <c r="AE28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF28" s="143" t="inlineStr">
+        <is>
+          <t>pendiente</t>
+        </is>
+      </c>
+      <c r="AG28" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AI28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AJ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AK28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AL28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AM28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AN28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO28" s="143" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AP28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="AR28" s="143" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="AS28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AT28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="AU28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AV28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AW28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AX28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AY28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="AZ28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BA28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BB28" s="143" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="BC28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BD28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BE28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BF28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BG28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BH28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BI28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BJ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BK28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BL28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BM28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BN28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BO28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BP28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BQ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BR28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BS28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BT28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BU28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BV28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BW28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="BX28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BY28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="BZ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CA28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CB28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CC28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CD28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CE28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CF28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CG28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CH28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CI28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CJ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CK28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CL28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CM28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CN28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CO28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CP28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CQ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CR28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CS28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="CT28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CU28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CV28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CW28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CX28" s="143" t="inlineStr">
+        <is>
+          <t>2021-01-26</t>
+        </is>
+      </c>
+      <c r="CY28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="CZ28" s="143" t="inlineStr">
+        <is>
+          <t>134530</t>
+        </is>
+      </c>
+      <c r="DA28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="DB28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DC28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DD28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DE28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DF28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DG28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DH28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DI28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DJ28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DK28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DL28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DM28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DN28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DO28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DP28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DQ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DR28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DS28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DT28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DU28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DV28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DW28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DX28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="DY28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="DZ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EA28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EB28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EC28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ED28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EE28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EF28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EG28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EH28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EI28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EJ28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EK28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EL28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EM28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EN28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EO28" s="143" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="EP28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EQ28" s="143" t="inlineStr">
+        <is>
+          <t>2021-03-23</t>
+        </is>
+      </c>
+      <c r="ER28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ES28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="ET28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="EU28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EV28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EW28" s="143" t="inlineStr">
+        <is>
+          <t>2021-01-25</t>
+        </is>
+      </c>
+      <c r="EX28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="EY28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="EZ28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FA28" s="143" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="FB28" s="143" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="FC28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FD28" s="143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="FE28" s="143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="FF28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FG28" s="143" t="inlineStr">
+        <is>
+          <t>1845-01-01</t>
+        </is>
+      </c>
+      <c r="FH28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FI28" s="143" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="FJ28" s="143" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
+        </is>
+      </c>
       <c r="FK28" s="143" t="n"/>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="73">

</xml_diff>

<commit_message>
[MODIFY] numero de ciclos en qt oral, correcion de ortografia de un medicamento oral
</commit_message>
<xml_diff>
--- a/prueba2.xlsx
+++ b/prueba2.xlsx
@@ -2228,7 +2228,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.71"/>
@@ -22598,7 +22598,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>